<commit_message>
Update grand canyon intervening to include Natural and USGS data
</commit_message>
<xml_diff>
--- a/InteractiveWaterBudget/InteractiveWaterBudget-CombinedPowellMead.xlsx
+++ b/InteractiveWaterBudget/InteractiveWaterBudget-CombinedPowellMead.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverFutures\InteractiveWaterBudget\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{349098B9-FE3C-4A1F-94F6-82DB5FB13C60}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFBBD286-A63E-449D-AE57-3143B97BEF78}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6640" activeTab="3" xr2:uid="{5373AB19-D84C-490D-97DC-C516D358024A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="166">
   <si>
     <t xml:space="preserve">    To Upper Basin</t>
   </si>
@@ -530,6 +530,9 @@
   <si>
     <t>Compare Upper Basin consumptive use for 9.0-Trade and 9.0-LawOfRiver</t>
   </si>
+  <si>
+    <t>4.9 to 6.5 feet per year for Powell, 5.5 to 6.4 feet per year from Schmidt et al (2016); 5.7 to 6.8 in Moreo (2015)</t>
+  </si>
 </sst>
 </file>
 
@@ -880,15 +883,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -902,6 +897,12 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -913,10 +914,12 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Accent2" xfId="6" builtinId="33"/>
@@ -927,207 +930,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="5" builtinId="5"/>
   </cellStyles>
-  <dxfs count="110">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="90">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -21879,20 +21682,20 @@
       <c r="D3"/>
     </row>
     <row r="4" spans="1:12" ht="164.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="51" t="s">
+      <c r="A4" s="62" t="s">
         <v>118</v>
       </c>
-      <c r="B4" s="51"/>
-      <c r="C4" s="51"/>
-      <c r="D4" s="51"/>
-      <c r="E4" s="51"/>
-      <c r="F4" s="51"/>
-      <c r="G4" s="51"/>
-      <c r="H4" s="51"/>
-      <c r="I4" s="51"/>
-      <c r="J4" s="51"/>
-      <c r="K4" s="51"/>
-      <c r="L4" s="51"/>
+      <c r="B4" s="62"/>
+      <c r="C4" s="62"/>
+      <c r="D4" s="62"/>
+      <c r="E4" s="62"/>
+      <c r="F4" s="62"/>
+      <c r="G4" s="62"/>
+      <c r="H4" s="62"/>
+      <c r="I4" s="62"/>
+      <c r="J4" s="62"/>
+      <c r="K4" s="62"/>
+      <c r="L4" s="62"/>
     </row>
     <row r="5" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="16"/>
@@ -21908,200 +21711,200 @@
       <c r="L5" s="16"/>
     </row>
     <row r="6" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="55" t="s">
+      <c r="A6" s="53" t="s">
         <v>123</v>
       </c>
-      <c r="B6" s="56"/>
-      <c r="C6" s="56"/>
-      <c r="D6" s="56"/>
-      <c r="E6" s="56"/>
-      <c r="F6" s="56"/>
-      <c r="G6" s="56"/>
-      <c r="H6" s="56"/>
-      <c r="I6" s="56"/>
-      <c r="J6" s="56"/>
-      <c r="K6" s="56"/>
-      <c r="L6" s="57"/>
+      <c r="B6" s="54"/>
+      <c r="C6" s="54"/>
+      <c r="D6" s="54"/>
+      <c r="E6" s="54"/>
+      <c r="F6" s="54"/>
+      <c r="G6" s="54"/>
+      <c r="H6" s="54"/>
+      <c r="I6" s="54"/>
+      <c r="J6" s="54"/>
+      <c r="K6" s="54"/>
+      <c r="L6" s="55"/>
     </row>
     <row r="7" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="29">
         <v>1</v>
       </c>
-      <c r="B7" s="52" t="s">
+      <c r="B7" s="56" t="s">
         <v>119</v>
       </c>
-      <c r="C7" s="52"/>
-      <c r="D7" s="52"/>
-      <c r="E7" s="52"/>
-      <c r="F7" s="52"/>
-      <c r="G7" s="52"/>
-      <c r="H7" s="52"/>
-      <c r="I7" s="52"/>
-      <c r="J7" s="52"/>
-      <c r="K7" s="52"/>
-      <c r="L7" s="53"/>
+      <c r="C7" s="56"/>
+      <c r="D7" s="56"/>
+      <c r="E7" s="56"/>
+      <c r="F7" s="56"/>
+      <c r="G7" s="56"/>
+      <c r="H7" s="56"/>
+      <c r="I7" s="56"/>
+      <c r="J7" s="56"/>
+      <c r="K7" s="56"/>
+      <c r="L7" s="57"/>
     </row>
     <row r="8" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="29">
         <v>2</v>
       </c>
-      <c r="B8" s="52" t="s">
+      <c r="B8" s="56" t="s">
         <v>99</v>
       </c>
-      <c r="C8" s="52"/>
-      <c r="D8" s="52"/>
-      <c r="E8" s="52"/>
-      <c r="F8" s="52"/>
-      <c r="G8" s="52"/>
-      <c r="H8" s="52"/>
-      <c r="I8" s="52"/>
-      <c r="J8" s="52"/>
-      <c r="K8" s="52"/>
-      <c r="L8" s="53"/>
+      <c r="C8" s="56"/>
+      <c r="D8" s="56"/>
+      <c r="E8" s="56"/>
+      <c r="F8" s="56"/>
+      <c r="G8" s="56"/>
+      <c r="H8" s="56"/>
+      <c r="I8" s="56"/>
+      <c r="J8" s="56"/>
+      <c r="K8" s="56"/>
+      <c r="L8" s="57"/>
     </row>
     <row r="9" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="29">
         <v>3</v>
       </c>
-      <c r="B9" s="52" t="s">
+      <c r="B9" s="56" t="s">
         <v>55</v>
       </c>
-      <c r="C9" s="52"/>
-      <c r="D9" s="52"/>
-      <c r="E9" s="52"/>
-      <c r="F9" s="52"/>
-      <c r="G9" s="52"/>
-      <c r="H9" s="52"/>
-      <c r="I9" s="52"/>
-      <c r="J9" s="52"/>
-      <c r="K9" s="52"/>
-      <c r="L9" s="53"/>
+      <c r="C9" s="56"/>
+      <c r="D9" s="56"/>
+      <c r="E9" s="56"/>
+      <c r="F9" s="56"/>
+      <c r="G9" s="56"/>
+      <c r="H9" s="56"/>
+      <c r="I9" s="56"/>
+      <c r="J9" s="56"/>
+      <c r="K9" s="56"/>
+      <c r="L9" s="57"/>
     </row>
     <row r="10" spans="1:12" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="29">
         <v>4</v>
       </c>
-      <c r="B10" s="52" t="s">
+      <c r="B10" s="56" t="s">
         <v>100</v>
       </c>
-      <c r="C10" s="52"/>
-      <c r="D10" s="52"/>
-      <c r="E10" s="52"/>
-      <c r="F10" s="52"/>
-      <c r="G10" s="52"/>
-      <c r="H10" s="52"/>
-      <c r="I10" s="52"/>
-      <c r="J10" s="52"/>
-      <c r="K10" s="52"/>
-      <c r="L10" s="53"/>
+      <c r="C10" s="56"/>
+      <c r="D10" s="56"/>
+      <c r="E10" s="56"/>
+      <c r="F10" s="56"/>
+      <c r="G10" s="56"/>
+      <c r="H10" s="56"/>
+      <c r="I10" s="56"/>
+      <c r="J10" s="56"/>
+      <c r="K10" s="56"/>
+      <c r="L10" s="57"/>
     </row>
     <row r="11" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="29">
         <v>5</v>
       </c>
-      <c r="B11" s="52" t="s">
+      <c r="B11" s="56" t="s">
         <v>57</v>
       </c>
-      <c r="C11" s="52"/>
-      <c r="D11" s="52"/>
-      <c r="E11" s="52"/>
-      <c r="F11" s="52"/>
-      <c r="G11" s="52"/>
-      <c r="H11" s="52"/>
-      <c r="I11" s="52"/>
-      <c r="J11" s="52"/>
-      <c r="K11" s="52"/>
-      <c r="L11" s="53"/>
+      <c r="C11" s="56"/>
+      <c r="D11" s="56"/>
+      <c r="E11" s="56"/>
+      <c r="F11" s="56"/>
+      <c r="G11" s="56"/>
+      <c r="H11" s="56"/>
+      <c r="I11" s="56"/>
+      <c r="J11" s="56"/>
+      <c r="K11" s="56"/>
+      <c r="L11" s="57"/>
     </row>
     <row r="12" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="29">
         <v>6</v>
       </c>
-      <c r="B12" s="52" t="s">
+      <c r="B12" s="56" t="s">
         <v>58</v>
       </c>
-      <c r="C12" s="52"/>
-      <c r="D12" s="52"/>
-      <c r="E12" s="52"/>
-      <c r="F12" s="52"/>
-      <c r="G12" s="52"/>
-      <c r="H12" s="52"/>
-      <c r="I12" s="52"/>
-      <c r="J12" s="52"/>
-      <c r="K12" s="52"/>
-      <c r="L12" s="53"/>
+      <c r="C12" s="56"/>
+      <c r="D12" s="56"/>
+      <c r="E12" s="56"/>
+      <c r="F12" s="56"/>
+      <c r="G12" s="56"/>
+      <c r="H12" s="56"/>
+      <c r="I12" s="56"/>
+      <c r="J12" s="56"/>
+      <c r="K12" s="56"/>
+      <c r="L12" s="57"/>
     </row>
     <row r="13" spans="1:12" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="29">
         <v>7</v>
       </c>
-      <c r="B13" s="52" t="s">
+      <c r="B13" s="56" t="s">
         <v>120</v>
       </c>
-      <c r="C13" s="52"/>
-      <c r="D13" s="52"/>
-      <c r="E13" s="52"/>
-      <c r="F13" s="52"/>
-      <c r="G13" s="52"/>
-      <c r="H13" s="52"/>
-      <c r="I13" s="52"/>
-      <c r="J13" s="52"/>
-      <c r="K13" s="52"/>
-      <c r="L13" s="53"/>
+      <c r="C13" s="56"/>
+      <c r="D13" s="56"/>
+      <c r="E13" s="56"/>
+      <c r="F13" s="56"/>
+      <c r="G13" s="56"/>
+      <c r="H13" s="56"/>
+      <c r="I13" s="56"/>
+      <c r="J13" s="56"/>
+      <c r="K13" s="56"/>
+      <c r="L13" s="57"/>
     </row>
     <row r="14" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="29">
         <v>8</v>
       </c>
-      <c r="B14" s="52" t="s">
+      <c r="B14" s="56" t="s">
         <v>121</v>
       </c>
-      <c r="C14" s="52"/>
-      <c r="D14" s="52"/>
-      <c r="E14" s="52"/>
-      <c r="F14" s="52"/>
-      <c r="G14" s="52"/>
-      <c r="H14" s="52"/>
-      <c r="I14" s="52"/>
-      <c r="J14" s="52"/>
-      <c r="K14" s="52"/>
-      <c r="L14" s="53"/>
+      <c r="C14" s="56"/>
+      <c r="D14" s="56"/>
+      <c r="E14" s="56"/>
+      <c r="F14" s="56"/>
+      <c r="G14" s="56"/>
+      <c r="H14" s="56"/>
+      <c r="I14" s="56"/>
+      <c r="J14" s="56"/>
+      <c r="K14" s="56"/>
+      <c r="L14" s="57"/>
     </row>
     <row r="15" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="29">
         <v>9</v>
       </c>
-      <c r="B15" s="52" t="s">
+      <c r="B15" s="56" t="s">
         <v>122</v>
       </c>
-      <c r="C15" s="52"/>
-      <c r="D15" s="52"/>
-      <c r="E15" s="52"/>
-      <c r="F15" s="52"/>
-      <c r="G15" s="52"/>
-      <c r="H15" s="52"/>
-      <c r="I15" s="52"/>
-      <c r="J15" s="52"/>
-      <c r="K15" s="52"/>
-      <c r="L15" s="53"/>
+      <c r="C15" s="56"/>
+      <c r="D15" s="56"/>
+      <c r="E15" s="56"/>
+      <c r="F15" s="56"/>
+      <c r="G15" s="56"/>
+      <c r="H15" s="56"/>
+      <c r="I15" s="56"/>
+      <c r="J15" s="56"/>
+      <c r="K15" s="56"/>
+      <c r="L15" s="57"/>
     </row>
     <row r="16" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="29">
         <v>10</v>
       </c>
-      <c r="B16" s="52" t="s">
+      <c r="B16" s="56" t="s">
         <v>59</v>
       </c>
-      <c r="C16" s="52"/>
-      <c r="D16" s="52"/>
-      <c r="E16" s="52"/>
-      <c r="F16" s="52"/>
-      <c r="G16" s="52"/>
-      <c r="H16" s="52"/>
-      <c r="I16" s="52"/>
-      <c r="J16" s="52"/>
-      <c r="K16" s="52"/>
-      <c r="L16" s="53"/>
+      <c r="C16" s="56"/>
+      <c r="D16" s="56"/>
+      <c r="E16" s="56"/>
+      <c r="F16" s="56"/>
+      <c r="G16" s="56"/>
+      <c r="H16" s="56"/>
+      <c r="I16" s="56"/>
+      <c r="J16" s="56"/>
+      <c r="K16" s="56"/>
+      <c r="L16" s="57"/>
     </row>
     <row r="17" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="29">
@@ -22219,23 +22022,28 @@
       </c>
     </row>
     <row r="31" spans="1:12" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="54" t="s">
+      <c r="A31" s="52" t="s">
         <v>124</v>
       </c>
-      <c r="B31" s="54"/>
-      <c r="C31" s="54"/>
-      <c r="D31" s="54"/>
-      <c r="E31" s="54"/>
-      <c r="F31" s="54"/>
-      <c r="G31" s="54"/>
-      <c r="H31" s="54"/>
-      <c r="I31" s="54"/>
-      <c r="J31" s="54"/>
-      <c r="K31" s="54"/>
-      <c r="L31" s="54"/>
+      <c r="B31" s="52"/>
+      <c r="C31" s="52"/>
+      <c r="D31" s="52"/>
+      <c r="E31" s="52"/>
+      <c r="F31" s="52"/>
+      <c r="G31" s="52"/>
+      <c r="H31" s="52"/>
+      <c r="I31" s="52"/>
+      <c r="J31" s="52"/>
+      <c r="K31" s="52"/>
+      <c r="L31" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A4:L4"/>
+    <mergeCell ref="B9:L9"/>
+    <mergeCell ref="B11:L11"/>
+    <mergeCell ref="B12:L12"/>
+    <mergeCell ref="B13:L13"/>
     <mergeCell ref="A31:L31"/>
     <mergeCell ref="A6:L6"/>
     <mergeCell ref="B10:L10"/>
@@ -22246,11 +22054,6 @@
     <mergeCell ref="B16:L16"/>
     <mergeCell ref="B17:L17"/>
     <mergeCell ref="B18:L18"/>
-    <mergeCell ref="A4:L4"/>
-    <mergeCell ref="B9:L9"/>
-    <mergeCell ref="B11:L11"/>
-    <mergeCell ref="B12:L12"/>
-    <mergeCell ref="B13:L13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -22324,48 +22127,48 @@
         <v>53</v>
       </c>
       <c r="B5" s="13"/>
-      <c r="C5" s="62"/>
-      <c r="D5" s="62"/>
-      <c r="E5" s="62"/>
-      <c r="F5" s="62"/>
-      <c r="G5" s="62"/>
-      <c r="H5" s="62"/>
+      <c r="C5" s="63"/>
+      <c r="D5" s="63"/>
+      <c r="E5" s="63"/>
+      <c r="F5" s="63"/>
+      <c r="G5" s="63"/>
+      <c r="H5" s="63"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="17" t="s">
         <v>41</v>
       </c>
       <c r="B6" s="13"/>
-      <c r="C6" s="62"/>
-      <c r="D6" s="62"/>
-      <c r="E6" s="62"/>
-      <c r="F6" s="62"/>
-      <c r="G6" s="62"/>
-      <c r="H6" s="62"/>
+      <c r="C6" s="63"/>
+      <c r="D6" s="63"/>
+      <c r="E6" s="63"/>
+      <c r="F6" s="63"/>
+      <c r="G6" s="63"/>
+      <c r="H6" s="63"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="17" t="s">
         <v>42</v>
       </c>
       <c r="B7" s="13"/>
-      <c r="C7" s="62"/>
-      <c r="D7" s="62"/>
-      <c r="E7" s="62"/>
-      <c r="F7" s="62"/>
-      <c r="G7" s="62"/>
-      <c r="H7" s="62"/>
+      <c r="C7" s="63"/>
+      <c r="D7" s="63"/>
+      <c r="E7" s="63"/>
+      <c r="F7" s="63"/>
+      <c r="G7" s="63"/>
+      <c r="H7" s="63"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="17" t="s">
         <v>43</v>
       </c>
       <c r="B8" s="13"/>
-      <c r="C8" s="62"/>
-      <c r="D8" s="62"/>
-      <c r="E8" s="62"/>
-      <c r="F8" s="62"/>
-      <c r="G8" s="62"/>
-      <c r="H8" s="62"/>
+      <c r="C8" s="63"/>
+      <c r="D8" s="63"/>
+      <c r="E8" s="63"/>
+      <c r="F8" s="63"/>
+      <c r="G8" s="63"/>
+      <c r="H8" s="63"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="17"/>
@@ -23487,7 +23290,7 @@
       <c r="F50" s="45"/>
       <c r="G50" s="45"/>
       <c r="H50" s="45">
-        <f t="shared" ref="E50:L50" si="17">G50</f>
+        <f t="shared" ref="H50:L50" si="17">G50</f>
         <v>0</v>
       </c>
       <c r="I50" s="45">
@@ -23532,7 +23335,7 @@
       <c r="F51" s="12"/>
       <c r="G51" s="12"/>
       <c r="H51" s="12">
-        <f t="shared" ref="D51:L51" si="18">IF(H$22&lt;&gt;"",0.6,"")</f>
+        <f t="shared" ref="H51:L51" si="18">IF(H$22&lt;&gt;"",0.6,"")</f>
         <v>0.6</v>
       </c>
       <c r="I51" s="12">
@@ -24002,172 +23805,172 @@
     <mergeCell ref="C8:H8"/>
   </mergeCells>
   <conditionalFormatting sqref="C49:L49">
-    <cfRule type="cellIs" dxfId="109" priority="44" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="89" priority="44" operator="greaterThan">
       <formula>$C$45</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:F49">
-    <cfRule type="cellIs" dxfId="108" priority="43" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="88" priority="43" operator="greaterThan">
       <formula>$C$45</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E49:F49">
-    <cfRule type="cellIs" dxfId="107" priority="42" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="87" priority="42" operator="greaterThan">
       <formula>$E$45</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D49:F49">
-    <cfRule type="cellIs" dxfId="106" priority="41" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="86" priority="41" operator="greaterThan">
       <formula>$D$45</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F49">
-    <cfRule type="cellIs" dxfId="105" priority="40" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="85" priority="40" operator="greaterThan">
       <formula>$F$45</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G49">
-    <cfRule type="cellIs" dxfId="104" priority="39" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="84" priority="39" operator="greaterThan">
       <formula>$G$45</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H49">
-    <cfRule type="cellIs" dxfId="103" priority="38" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="83" priority="38" operator="greaterThan">
       <formula>$H$45</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I49">
-    <cfRule type="cellIs" dxfId="102" priority="37" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="82" priority="37" operator="greaterThan">
       <formula>$I$45</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J49">
-    <cfRule type="cellIs" dxfId="101" priority="36" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="81" priority="36" operator="greaterThan">
       <formula>$J$45</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K49">
-    <cfRule type="cellIs" dxfId="100" priority="35" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="80" priority="35" operator="greaterThan">
       <formula>$K$45</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L49">
-    <cfRule type="cellIs" dxfId="99" priority="34" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="79" priority="34" operator="greaterThan">
       <formula>$L$45</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H50:L50">
-    <cfRule type="cellIs" dxfId="97" priority="32" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="78" priority="32" operator="greaterThan">
       <formula>$D$46</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H50">
-    <cfRule type="cellIs" dxfId="92" priority="27" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="77" priority="27" operator="greaterThan">
       <formula>$H$46</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I50">
-    <cfRule type="cellIs" dxfId="91" priority="26" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="76" priority="26" operator="greaterThan">
       <formula>$I$46</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J50">
-    <cfRule type="cellIs" dxfId="90" priority="25" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="75" priority="25" operator="greaterThan">
       <formula>$J$46</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K50">
-    <cfRule type="cellIs" dxfId="89" priority="24" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="74" priority="24" operator="greaterThan">
       <formula>$K$46</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L50">
-    <cfRule type="cellIs" dxfId="88" priority="23" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="73" priority="23" operator="greaterThan">
       <formula>$L$46</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H52">
-    <cfRule type="cellIs" dxfId="82" priority="17" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="72" priority="17" operator="greaterThan">
       <formula>$H$47</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I52">
-    <cfRule type="cellIs" dxfId="81" priority="16" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="71" priority="16" operator="greaterThan">
       <formula>$I$47</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J52">
-    <cfRule type="cellIs" dxfId="80" priority="15" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="70" priority="15" operator="greaterThan">
       <formula>$J$47</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K52">
-    <cfRule type="cellIs" dxfId="79" priority="14" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="69" priority="14" operator="greaterThan">
       <formula>$K$47</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L52">
-    <cfRule type="cellIs" dxfId="78" priority="13" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="68" priority="13" operator="greaterThan">
       <formula>$L$47</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C50:G50">
-    <cfRule type="cellIs" dxfId="77" priority="12" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="67" priority="12" operator="greaterThan">
       <formula>$C$45</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C50:F50">
-    <cfRule type="cellIs" dxfId="76" priority="11" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="66" priority="11" operator="greaterThan">
       <formula>$C$45</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E50:F50">
-    <cfRule type="cellIs" dxfId="75" priority="10" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="65" priority="10" operator="greaterThan">
       <formula>$E$45</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D50:F50">
-    <cfRule type="cellIs" dxfId="74" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="64" priority="9" operator="greaterThan">
       <formula>$D$45</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F50">
-    <cfRule type="cellIs" dxfId="73" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="63" priority="8" operator="greaterThan">
       <formula>$F$45</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G50">
-    <cfRule type="cellIs" dxfId="72" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="62" priority="7" operator="greaterThan">
       <formula>$G$45</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C52:G52">
-    <cfRule type="cellIs" dxfId="71" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="61" priority="6" operator="greaterThan">
       <formula>$C$45</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C52:F52">
-    <cfRule type="cellIs" dxfId="70" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="60" priority="5" operator="greaterThan">
       <formula>$C$45</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E52:F52">
-    <cfRule type="cellIs" dxfId="69" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="59" priority="4" operator="greaterThan">
       <formula>$E$45</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D52:F52">
-    <cfRule type="cellIs" dxfId="68" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="58" priority="3" operator="greaterThan">
       <formula>$D$45</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F52">
-    <cfRule type="cellIs" dxfId="67" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="57" priority="2" operator="greaterThan">
       <formula>$F$45</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G52">
-    <cfRule type="cellIs" dxfId="66" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="56" priority="1" operator="greaterThan">
       <formula>$G$45</formula>
     </cfRule>
   </conditionalFormatting>
@@ -24243,48 +24046,48 @@
         <v>53</v>
       </c>
       <c r="B5" s="50"/>
-      <c r="C5" s="62"/>
-      <c r="D5" s="62"/>
-      <c r="E5" s="62"/>
-      <c r="F5" s="62"/>
-      <c r="G5" s="62"/>
-      <c r="H5" s="62"/>
+      <c r="C5" s="63"/>
+      <c r="D5" s="63"/>
+      <c r="E5" s="63"/>
+      <c r="F5" s="63"/>
+      <c r="G5" s="63"/>
+      <c r="H5" s="63"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="17" t="s">
         <v>41</v>
       </c>
       <c r="B6" s="50"/>
-      <c r="C6" s="62"/>
-      <c r="D6" s="62"/>
-      <c r="E6" s="62"/>
-      <c r="F6" s="62"/>
-      <c r="G6" s="62"/>
-      <c r="H6" s="62"/>
+      <c r="C6" s="63"/>
+      <c r="D6" s="63"/>
+      <c r="E6" s="63"/>
+      <c r="F6" s="63"/>
+      <c r="G6" s="63"/>
+      <c r="H6" s="63"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="17" t="s">
         <v>42</v>
       </c>
       <c r="B7" s="50"/>
-      <c r="C7" s="62"/>
-      <c r="D7" s="62"/>
-      <c r="E7" s="62"/>
-      <c r="F7" s="62"/>
-      <c r="G7" s="62"/>
-      <c r="H7" s="62"/>
+      <c r="C7" s="63"/>
+      <c r="D7" s="63"/>
+      <c r="E7" s="63"/>
+      <c r="F7" s="63"/>
+      <c r="G7" s="63"/>
+      <c r="H7" s="63"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="17" t="s">
         <v>43</v>
       </c>
       <c r="B8" s="50"/>
-      <c r="C8" s="62"/>
-      <c r="D8" s="62"/>
-      <c r="E8" s="62"/>
-      <c r="F8" s="62"/>
-      <c r="G8" s="62"/>
-      <c r="H8" s="62"/>
+      <c r="C8" s="63"/>
+      <c r="D8" s="63"/>
+      <c r="E8" s="63"/>
+      <c r="F8" s="63"/>
+      <c r="G8" s="63"/>
+      <c r="H8" s="63"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="17"/>
@@ -26006,160 +25809,160 @@
     <mergeCell ref="C8:H8"/>
   </mergeCells>
   <conditionalFormatting sqref="C49:L49">
-    <cfRule type="cellIs" dxfId="65" priority="32" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="55" priority="32" operator="greaterThan">
       <formula>$C$45</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:F49">
-    <cfRule type="cellIs" dxfId="64" priority="31" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="54" priority="31" operator="greaterThan">
       <formula>$C$45</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E49:F49">
-    <cfRule type="cellIs" dxfId="63" priority="30" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="53" priority="30" operator="greaterThan">
       <formula>$E$45</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D49:F49">
-    <cfRule type="cellIs" dxfId="62" priority="29" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="52" priority="29" operator="greaterThan">
       <formula>$D$45</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F49">
-    <cfRule type="cellIs" dxfId="61" priority="28" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="51" priority="28" operator="greaterThan">
       <formula>$F$45</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G49">
-    <cfRule type="cellIs" dxfId="60" priority="27" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="50" priority="27" operator="greaterThan">
       <formula>$G$45</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H49">
-    <cfRule type="cellIs" dxfId="59" priority="26" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="49" priority="26" operator="greaterThan">
       <formula>$H$45</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I49">
-    <cfRule type="cellIs" dxfId="58" priority="25" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="48" priority="25" operator="greaterThan">
       <formula>$I$45</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J49">
-    <cfRule type="cellIs" dxfId="57" priority="24" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="47" priority="24" operator="greaterThan">
       <formula>$J$45</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K49">
-    <cfRule type="cellIs" dxfId="56" priority="23" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="46" priority="23" operator="greaterThan">
       <formula>$K$45</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L49">
-    <cfRule type="cellIs" dxfId="55" priority="22" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="45" priority="22" operator="greaterThan">
       <formula>$L$45</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C50">
-    <cfRule type="cellIs" dxfId="54" priority="21" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="44" priority="21" operator="greaterThan">
       <formula>$C$46</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D50:L50">
-    <cfRule type="cellIs" dxfId="53" priority="20" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="43" priority="20" operator="greaterThan">
       <formula>$D$46</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E50">
-    <cfRule type="cellIs" dxfId="52" priority="19" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="42" priority="19" operator="greaterThan">
       <formula>$E$46</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F50">
-    <cfRule type="cellIs" dxfId="51" priority="18" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="41" priority="18" operator="greaterThan">
       <formula>$F$46</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G50">
-    <cfRule type="cellIs" dxfId="50" priority="16" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="40" priority="16" operator="greaterThan">
       <formula>$G$46</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="17" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="39" priority="17" operator="greaterThan">
       <formula>$G$46</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H50">
-    <cfRule type="cellIs" dxfId="48" priority="15" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="38" priority="15" operator="greaterThan">
       <formula>$H$46</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I50">
-    <cfRule type="cellIs" dxfId="47" priority="14" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="37" priority="14" operator="greaterThan">
       <formula>$I$46</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J50">
-    <cfRule type="cellIs" dxfId="46" priority="13" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="36" priority="13" operator="greaterThan">
       <formula>$J$46</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K50">
-    <cfRule type="cellIs" dxfId="45" priority="12" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="35" priority="12" operator="greaterThan">
       <formula>$K$46</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L50">
-    <cfRule type="cellIs" dxfId="44" priority="11" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="34" priority="11" operator="greaterThan">
       <formula>$L$46</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C52">
-    <cfRule type="cellIs" dxfId="43" priority="10" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="33" priority="10" operator="greaterThan">
       <formula>$C$47</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D52">
-    <cfRule type="cellIs" dxfId="42" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="32" priority="9" operator="greaterThan">
       <formula>$D$47</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E52">
-    <cfRule type="cellIs" dxfId="41" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="31" priority="8" operator="greaterThan">
       <formula>$E$47</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F52">
-    <cfRule type="cellIs" dxfId="40" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="30" priority="7" operator="greaterThan">
       <formula>$F$47</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G52">
-    <cfRule type="cellIs" dxfId="39" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="29" priority="6" operator="greaterThan">
       <formula>$G$47</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H52">
-    <cfRule type="cellIs" dxfId="38" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="28" priority="5" operator="greaterThan">
       <formula>$H$47</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I52">
-    <cfRule type="cellIs" dxfId="37" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="27" priority="4" operator="greaterThan">
       <formula>$I$47</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J52">
-    <cfRule type="cellIs" dxfId="36" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="26" priority="3" operator="greaterThan">
       <formula>$J$47</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K52">
-    <cfRule type="cellIs" dxfId="35" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="25" priority="2" operator="greaterThan">
       <formula>$K$47</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L52">
-    <cfRule type="cellIs" dxfId="34" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="24" priority="1" operator="greaterThan">
       <formula>$L$47</formula>
     </cfRule>
   </conditionalFormatting>
@@ -26172,7 +25975,7 @@
   <dimension ref="A1:R62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -26235,48 +26038,48 @@
         <v>53</v>
       </c>
       <c r="B5" s="50"/>
-      <c r="C5" s="62"/>
-      <c r="D5" s="62"/>
-      <c r="E5" s="62"/>
-      <c r="F5" s="62"/>
-      <c r="G5" s="62"/>
-      <c r="H5" s="62"/>
+      <c r="C5" s="63"/>
+      <c r="D5" s="63"/>
+      <c r="E5" s="63"/>
+      <c r="F5" s="63"/>
+      <c r="G5" s="63"/>
+      <c r="H5" s="63"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="17" t="s">
         <v>41</v>
       </c>
       <c r="B6" s="50"/>
-      <c r="C6" s="62"/>
-      <c r="D6" s="62"/>
-      <c r="E6" s="62"/>
-      <c r="F6" s="62"/>
-      <c r="G6" s="62"/>
-      <c r="H6" s="62"/>
+      <c r="C6" s="63"/>
+      <c r="D6" s="63"/>
+      <c r="E6" s="63"/>
+      <c r="F6" s="63"/>
+      <c r="G6" s="63"/>
+      <c r="H6" s="63"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="17" t="s">
         <v>42</v>
       </c>
       <c r="B7" s="50"/>
-      <c r="C7" s="62"/>
-      <c r="D7" s="62"/>
-      <c r="E7" s="62"/>
-      <c r="F7" s="62"/>
-      <c r="G7" s="62"/>
-      <c r="H7" s="62"/>
+      <c r="C7" s="63"/>
+      <c r="D7" s="63"/>
+      <c r="E7" s="63"/>
+      <c r="F7" s="63"/>
+      <c r="G7" s="63"/>
+      <c r="H7" s="63"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="17" t="s">
         <v>43</v>
       </c>
       <c r="B8" s="50"/>
-      <c r="C8" s="62"/>
-      <c r="D8" s="62"/>
-      <c r="E8" s="62"/>
-      <c r="F8" s="62"/>
-      <c r="G8" s="62"/>
-      <c r="H8" s="62"/>
+      <c r="C8" s="63"/>
+      <c r="D8" s="63"/>
+      <c r="E8" s="63"/>
+      <c r="F8" s="63"/>
+      <c r="G8" s="63"/>
+      <c r="H8" s="63"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="17"/>
@@ -26334,7 +26137,7 @@
         <v>6</v>
       </c>
       <c r="D18" s="24" t="s">
-        <v>129</v>
+        <v>165</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.35">
@@ -27413,7 +27216,7 @@
       <c r="L49" s="45">
         <v>2</v>
       </c>
-      <c r="M49" s="63"/>
+      <c r="M49" s="51"/>
       <c r="N49" s="1" t="s">
         <v>144</v>
       </c>
@@ -27443,7 +27246,7 @@
         <v>6.7829999999999995</v>
       </c>
       <c r="H50" s="45">
-        <f t="shared" ref="E50:L50" si="16">G50</f>
+        <f t="shared" ref="H50:L50" si="16">G50</f>
         <v>6.7829999999999995</v>
       </c>
       <c r="I50" s="45">
@@ -27983,37 +27786,37 @@
     <mergeCell ref="C8:H8"/>
   </mergeCells>
   <conditionalFormatting sqref="H49:L49">
-    <cfRule type="cellIs" dxfId="33" priority="33" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="23" priority="33" operator="greaterThan">
       <formula>$C$45</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H49">
-    <cfRule type="cellIs" dxfId="27" priority="27" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="22" priority="27" operator="greaterThan">
       <formula>$H$45</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I49">
-    <cfRule type="cellIs" dxfId="26" priority="26" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="21" priority="26" operator="greaterThan">
       <formula>$I$45</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J49">
-    <cfRule type="cellIs" dxfId="25" priority="25" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="20" priority="25" operator="greaterThan">
       <formula>$J$45</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K49">
-    <cfRule type="cellIs" dxfId="24" priority="24" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="19" priority="24" operator="greaterThan">
       <formula>$K$45</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L49">
-    <cfRule type="cellIs" dxfId="23" priority="23" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="18" priority="23" operator="greaterThan">
       <formula>$L$45</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H50:L50">
-    <cfRule type="cellIs" dxfId="21" priority="21" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="17" priority="21" operator="greaterThan">
       <formula>$D$46</formula>
     </cfRule>
   </conditionalFormatting>
@@ -28169,48 +27972,48 @@
         <v>53</v>
       </c>
       <c r="B5" s="36"/>
-      <c r="C5" s="62"/>
-      <c r="D5" s="62"/>
-      <c r="E5" s="62"/>
-      <c r="F5" s="62"/>
-      <c r="G5" s="62"/>
-      <c r="H5" s="62"/>
+      <c r="C5" s="63"/>
+      <c r="D5" s="63"/>
+      <c r="E5" s="63"/>
+      <c r="F5" s="63"/>
+      <c r="G5" s="63"/>
+      <c r="H5" s="63"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="17" t="s">
         <v>41</v>
       </c>
       <c r="B6" s="36"/>
-      <c r="C6" s="62"/>
-      <c r="D6" s="62"/>
-      <c r="E6" s="62"/>
-      <c r="F6" s="62"/>
-      <c r="G6" s="62"/>
-      <c r="H6" s="62"/>
+      <c r="C6" s="63"/>
+      <c r="D6" s="63"/>
+      <c r="E6" s="63"/>
+      <c r="F6" s="63"/>
+      <c r="G6" s="63"/>
+      <c r="H6" s="63"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="17" t="s">
         <v>42</v>
       </c>
       <c r="B7" s="36"/>
-      <c r="C7" s="62"/>
-      <c r="D7" s="62"/>
-      <c r="E7" s="62"/>
-      <c r="F7" s="62"/>
-      <c r="G7" s="62"/>
-      <c r="H7" s="62"/>
+      <c r="C7" s="63"/>
+      <c r="D7" s="63"/>
+      <c r="E7" s="63"/>
+      <c r="F7" s="63"/>
+      <c r="G7" s="63"/>
+      <c r="H7" s="63"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="17" t="s">
         <v>43</v>
       </c>
       <c r="B8" s="36"/>
-      <c r="C8" s="62"/>
-      <c r="D8" s="62"/>
-      <c r="E8" s="62"/>
-      <c r="F8" s="62"/>
-      <c r="G8" s="62"/>
-      <c r="H8" s="62"/>
+      <c r="C8" s="63"/>
+      <c r="D8" s="63"/>
+      <c r="E8" s="63"/>
+      <c r="F8" s="63"/>
+      <c r="G8" s="63"/>
+      <c r="H8" s="63"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="17"/>

</xml_diff>

<commit_message>
Update readme Time to Mead Dead pool. Add some parameters for sensitivity analysis
</commit_message>
<xml_diff>
--- a/InteractiveWaterBudget/InteractiveWaterBudget-CombinedPowellMead.xlsx
+++ b/InteractiveWaterBudget/InteractiveWaterBudget-CombinedPowellMead.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverFutures\InteractiveWaterBudget\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFBBD286-A63E-449D-AE57-3143B97BEF78}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C730CF91-40C5-4824-90A6-A940BEC7D12E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6640" activeTab="3" xr2:uid="{5373AB19-D84C-490D-97DC-C516D358024A}"/>
   </bookViews>
@@ -884,6 +884,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -897,12 +906,6 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -913,9 +916,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -21682,20 +21682,20 @@
       <c r="D3"/>
     </row>
     <row r="4" spans="1:12" ht="164.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="62" t="s">
+      <c r="A4" s="52" t="s">
         <v>118</v>
       </c>
-      <c r="B4" s="62"/>
-      <c r="C4" s="62"/>
-      <c r="D4" s="62"/>
-      <c r="E4" s="62"/>
-      <c r="F4" s="62"/>
-      <c r="G4" s="62"/>
-      <c r="H4" s="62"/>
-      <c r="I4" s="62"/>
-      <c r="J4" s="62"/>
-      <c r="K4" s="62"/>
-      <c r="L4" s="62"/>
+      <c r="B4" s="52"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="52"/>
+      <c r="G4" s="52"/>
+      <c r="H4" s="52"/>
+      <c r="I4" s="52"/>
+      <c r="J4" s="52"/>
+      <c r="K4" s="52"/>
+      <c r="L4" s="52"/>
     </row>
     <row r="5" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="16"/>
@@ -21711,236 +21711,236 @@
       <c r="L5" s="16"/>
     </row>
     <row r="6" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="53" t="s">
+      <c r="A6" s="56" t="s">
         <v>123</v>
       </c>
-      <c r="B6" s="54"/>
-      <c r="C6" s="54"/>
-      <c r="D6" s="54"/>
-      <c r="E6" s="54"/>
-      <c r="F6" s="54"/>
-      <c r="G6" s="54"/>
-      <c r="H6" s="54"/>
-      <c r="I6" s="54"/>
-      <c r="J6" s="54"/>
-      <c r="K6" s="54"/>
-      <c r="L6" s="55"/>
+      <c r="B6" s="57"/>
+      <c r="C6" s="57"/>
+      <c r="D6" s="57"/>
+      <c r="E6" s="57"/>
+      <c r="F6" s="57"/>
+      <c r="G6" s="57"/>
+      <c r="H6" s="57"/>
+      <c r="I6" s="57"/>
+      <c r="J6" s="57"/>
+      <c r="K6" s="57"/>
+      <c r="L6" s="58"/>
     </row>
     <row r="7" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="29">
         <v>1</v>
       </c>
-      <c r="B7" s="56" t="s">
+      <c r="B7" s="53" t="s">
         <v>119</v>
       </c>
-      <c r="C7" s="56"/>
-      <c r="D7" s="56"/>
-      <c r="E7" s="56"/>
-      <c r="F7" s="56"/>
-      <c r="G7" s="56"/>
-      <c r="H7" s="56"/>
-      <c r="I7" s="56"/>
-      <c r="J7" s="56"/>
-      <c r="K7" s="56"/>
-      <c r="L7" s="57"/>
+      <c r="C7" s="53"/>
+      <c r="D7" s="53"/>
+      <c r="E7" s="53"/>
+      <c r="F7" s="53"/>
+      <c r="G7" s="53"/>
+      <c r="H7" s="53"/>
+      <c r="I7" s="53"/>
+      <c r="J7" s="53"/>
+      <c r="K7" s="53"/>
+      <c r="L7" s="54"/>
     </row>
     <row r="8" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="29">
         <v>2</v>
       </c>
-      <c r="B8" s="56" t="s">
+      <c r="B8" s="53" t="s">
         <v>99</v>
       </c>
-      <c r="C8" s="56"/>
-      <c r="D8" s="56"/>
-      <c r="E8" s="56"/>
-      <c r="F8" s="56"/>
-      <c r="G8" s="56"/>
-      <c r="H8" s="56"/>
-      <c r="I8" s="56"/>
-      <c r="J8" s="56"/>
-      <c r="K8" s="56"/>
-      <c r="L8" s="57"/>
+      <c r="C8" s="53"/>
+      <c r="D8" s="53"/>
+      <c r="E8" s="53"/>
+      <c r="F8" s="53"/>
+      <c r="G8" s="53"/>
+      <c r="H8" s="53"/>
+      <c r="I8" s="53"/>
+      <c r="J8" s="53"/>
+      <c r="K8" s="53"/>
+      <c r="L8" s="54"/>
     </row>
     <row r="9" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="29">
         <v>3</v>
       </c>
-      <c r="B9" s="56" t="s">
+      <c r="B9" s="53" t="s">
         <v>55</v>
       </c>
-      <c r="C9" s="56"/>
-      <c r="D9" s="56"/>
-      <c r="E9" s="56"/>
-      <c r="F9" s="56"/>
-      <c r="G9" s="56"/>
-      <c r="H9" s="56"/>
-      <c r="I9" s="56"/>
-      <c r="J9" s="56"/>
-      <c r="K9" s="56"/>
-      <c r="L9" s="57"/>
+      <c r="C9" s="53"/>
+      <c r="D9" s="53"/>
+      <c r="E9" s="53"/>
+      <c r="F9" s="53"/>
+      <c r="G9" s="53"/>
+      <c r="H9" s="53"/>
+      <c r="I9" s="53"/>
+      <c r="J9" s="53"/>
+      <c r="K9" s="53"/>
+      <c r="L9" s="54"/>
     </row>
     <row r="10" spans="1:12" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="29">
         <v>4</v>
       </c>
-      <c r="B10" s="56" t="s">
+      <c r="B10" s="53" t="s">
         <v>100</v>
       </c>
-      <c r="C10" s="56"/>
-      <c r="D10" s="56"/>
-      <c r="E10" s="56"/>
-      <c r="F10" s="56"/>
-      <c r="G10" s="56"/>
-      <c r="H10" s="56"/>
-      <c r="I10" s="56"/>
-      <c r="J10" s="56"/>
-      <c r="K10" s="56"/>
-      <c r="L10" s="57"/>
+      <c r="C10" s="53"/>
+      <c r="D10" s="53"/>
+      <c r="E10" s="53"/>
+      <c r="F10" s="53"/>
+      <c r="G10" s="53"/>
+      <c r="H10" s="53"/>
+      <c r="I10" s="53"/>
+      <c r="J10" s="53"/>
+      <c r="K10" s="53"/>
+      <c r="L10" s="54"/>
     </row>
     <row r="11" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="29">
         <v>5</v>
       </c>
-      <c r="B11" s="56" t="s">
+      <c r="B11" s="53" t="s">
         <v>57</v>
       </c>
-      <c r="C11" s="56"/>
-      <c r="D11" s="56"/>
-      <c r="E11" s="56"/>
-      <c r="F11" s="56"/>
-      <c r="G11" s="56"/>
-      <c r="H11" s="56"/>
-      <c r="I11" s="56"/>
-      <c r="J11" s="56"/>
-      <c r="K11" s="56"/>
-      <c r="L11" s="57"/>
+      <c r="C11" s="53"/>
+      <c r="D11" s="53"/>
+      <c r="E11" s="53"/>
+      <c r="F11" s="53"/>
+      <c r="G11" s="53"/>
+      <c r="H11" s="53"/>
+      <c r="I11" s="53"/>
+      <c r="J11" s="53"/>
+      <c r="K11" s="53"/>
+      <c r="L11" s="54"/>
     </row>
     <row r="12" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="29">
         <v>6</v>
       </c>
-      <c r="B12" s="56" t="s">
+      <c r="B12" s="53" t="s">
         <v>58</v>
       </c>
-      <c r="C12" s="56"/>
-      <c r="D12" s="56"/>
-      <c r="E12" s="56"/>
-      <c r="F12" s="56"/>
-      <c r="G12" s="56"/>
-      <c r="H12" s="56"/>
-      <c r="I12" s="56"/>
-      <c r="J12" s="56"/>
-      <c r="K12" s="56"/>
-      <c r="L12" s="57"/>
+      <c r="C12" s="53"/>
+      <c r="D12" s="53"/>
+      <c r="E12" s="53"/>
+      <c r="F12" s="53"/>
+      <c r="G12" s="53"/>
+      <c r="H12" s="53"/>
+      <c r="I12" s="53"/>
+      <c r="J12" s="53"/>
+      <c r="K12" s="53"/>
+      <c r="L12" s="54"/>
     </row>
     <row r="13" spans="1:12" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="29">
         <v>7</v>
       </c>
-      <c r="B13" s="56" t="s">
+      <c r="B13" s="53" t="s">
         <v>120</v>
       </c>
-      <c r="C13" s="56"/>
-      <c r="D13" s="56"/>
-      <c r="E13" s="56"/>
-      <c r="F13" s="56"/>
-      <c r="G13" s="56"/>
-      <c r="H13" s="56"/>
-      <c r="I13" s="56"/>
-      <c r="J13" s="56"/>
-      <c r="K13" s="56"/>
-      <c r="L13" s="57"/>
+      <c r="C13" s="53"/>
+      <c r="D13" s="53"/>
+      <c r="E13" s="53"/>
+      <c r="F13" s="53"/>
+      <c r="G13" s="53"/>
+      <c r="H13" s="53"/>
+      <c r="I13" s="53"/>
+      <c r="J13" s="53"/>
+      <c r="K13" s="53"/>
+      <c r="L13" s="54"/>
     </row>
     <row r="14" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="29">
         <v>8</v>
       </c>
-      <c r="B14" s="56" t="s">
+      <c r="B14" s="53" t="s">
         <v>121</v>
       </c>
-      <c r="C14" s="56"/>
-      <c r="D14" s="56"/>
-      <c r="E14" s="56"/>
-      <c r="F14" s="56"/>
-      <c r="G14" s="56"/>
-      <c r="H14" s="56"/>
-      <c r="I14" s="56"/>
-      <c r="J14" s="56"/>
-      <c r="K14" s="56"/>
-      <c r="L14" s="57"/>
+      <c r="C14" s="53"/>
+      <c r="D14" s="53"/>
+      <c r="E14" s="53"/>
+      <c r="F14" s="53"/>
+      <c r="G14" s="53"/>
+      <c r="H14" s="53"/>
+      <c r="I14" s="53"/>
+      <c r="J14" s="53"/>
+      <c r="K14" s="53"/>
+      <c r="L14" s="54"/>
     </row>
     <row r="15" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="29">
         <v>9</v>
       </c>
-      <c r="B15" s="56" t="s">
+      <c r="B15" s="53" t="s">
         <v>122</v>
       </c>
-      <c r="C15" s="56"/>
-      <c r="D15" s="56"/>
-      <c r="E15" s="56"/>
-      <c r="F15" s="56"/>
-      <c r="G15" s="56"/>
-      <c r="H15" s="56"/>
-      <c r="I15" s="56"/>
-      <c r="J15" s="56"/>
-      <c r="K15" s="56"/>
-      <c r="L15" s="57"/>
+      <c r="C15" s="53"/>
+      <c r="D15" s="53"/>
+      <c r="E15" s="53"/>
+      <c r="F15" s="53"/>
+      <c r="G15" s="53"/>
+      <c r="H15" s="53"/>
+      <c r="I15" s="53"/>
+      <c r="J15" s="53"/>
+      <c r="K15" s="53"/>
+      <c r="L15" s="54"/>
     </row>
     <row r="16" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="29">
         <v>10</v>
       </c>
-      <c r="B16" s="56" t="s">
+      <c r="B16" s="53" t="s">
         <v>59</v>
       </c>
-      <c r="C16" s="56"/>
-      <c r="D16" s="56"/>
-      <c r="E16" s="56"/>
-      <c r="F16" s="56"/>
-      <c r="G16" s="56"/>
-      <c r="H16" s="56"/>
-      <c r="I16" s="56"/>
-      <c r="J16" s="56"/>
-      <c r="K16" s="56"/>
-      <c r="L16" s="57"/>
+      <c r="C16" s="53"/>
+      <c r="D16" s="53"/>
+      <c r="E16" s="53"/>
+      <c r="F16" s="53"/>
+      <c r="G16" s="53"/>
+      <c r="H16" s="53"/>
+      <c r="I16" s="53"/>
+      <c r="J16" s="53"/>
+      <c r="K16" s="53"/>
+      <c r="L16" s="54"/>
     </row>
     <row r="17" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="29">
         <v>11</v>
       </c>
-      <c r="B17" s="58" t="s">
+      <c r="B17" s="59" t="s">
         <v>60</v>
       </c>
-      <c r="C17" s="58"/>
-      <c r="D17" s="58"/>
-      <c r="E17" s="58"/>
-      <c r="F17" s="58"/>
-      <c r="G17" s="58"/>
-      <c r="H17" s="58"/>
-      <c r="I17" s="58"/>
-      <c r="J17" s="58"/>
-      <c r="K17" s="58"/>
-      <c r="L17" s="59"/>
+      <c r="C17" s="59"/>
+      <c r="D17" s="59"/>
+      <c r="E17" s="59"/>
+      <c r="F17" s="59"/>
+      <c r="G17" s="59"/>
+      <c r="H17" s="59"/>
+      <c r="I17" s="59"/>
+      <c r="J17" s="59"/>
+      <c r="K17" s="59"/>
+      <c r="L17" s="60"/>
     </row>
     <row r="18" spans="1:12" ht="32" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="29">
         <v>12</v>
       </c>
-      <c r="B18" s="60" t="s">
+      <c r="B18" s="61" t="s">
         <v>108</v>
       </c>
-      <c r="C18" s="60"/>
-      <c r="D18" s="60"/>
-      <c r="E18" s="60"/>
-      <c r="F18" s="60"/>
-      <c r="G18" s="60"/>
-      <c r="H18" s="60"/>
-      <c r="I18" s="60"/>
-      <c r="J18" s="60"/>
-      <c r="K18" s="60"/>
-      <c r="L18" s="61"/>
+      <c r="C18" s="61"/>
+      <c r="D18" s="61"/>
+      <c r="E18" s="61"/>
+      <c r="F18" s="61"/>
+      <c r="G18" s="61"/>
+      <c r="H18" s="61"/>
+      <c r="I18" s="61"/>
+      <c r="J18" s="61"/>
+      <c r="K18" s="61"/>
+      <c r="L18" s="62"/>
     </row>
     <row r="19" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B19" s="27"/>
@@ -22022,28 +22022,23 @@
       </c>
     </row>
     <row r="31" spans="1:12" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="52" t="s">
+      <c r="A31" s="55" t="s">
         <v>124</v>
       </c>
-      <c r="B31" s="52"/>
-      <c r="C31" s="52"/>
-      <c r="D31" s="52"/>
-      <c r="E31" s="52"/>
-      <c r="F31" s="52"/>
-      <c r="G31" s="52"/>
-      <c r="H31" s="52"/>
-      <c r="I31" s="52"/>
-      <c r="J31" s="52"/>
-      <c r="K31" s="52"/>
-      <c r="L31" s="52"/>
+      <c r="B31" s="55"/>
+      <c r="C31" s="55"/>
+      <c r="D31" s="55"/>
+      <c r="E31" s="55"/>
+      <c r="F31" s="55"/>
+      <c r="G31" s="55"/>
+      <c r="H31" s="55"/>
+      <c r="I31" s="55"/>
+      <c r="J31" s="55"/>
+      <c r="K31" s="55"/>
+      <c r="L31" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A4:L4"/>
-    <mergeCell ref="B9:L9"/>
-    <mergeCell ref="B11:L11"/>
-    <mergeCell ref="B12:L12"/>
-    <mergeCell ref="B13:L13"/>
     <mergeCell ref="A31:L31"/>
     <mergeCell ref="A6:L6"/>
     <mergeCell ref="B10:L10"/>
@@ -22054,6 +22049,11 @@
     <mergeCell ref="B16:L16"/>
     <mergeCell ref="B17:L17"/>
     <mergeCell ref="B18:L18"/>
+    <mergeCell ref="A4:L4"/>
+    <mergeCell ref="B9:L9"/>
+    <mergeCell ref="B11:L11"/>
+    <mergeCell ref="B12:L12"/>
+    <mergeCell ref="B13:L13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update combined to 11 maf event; Move all but one spreadsheet to OlderVersions
</commit_message>
<xml_diff>
--- a/InteractiveWaterBudget/InteractiveWaterBudget-CombinedPowellMead.xlsx
+++ b/InteractiveWaterBudget/InteractiveWaterBudget-CombinedPowellMead.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverFutures\InteractiveWaterBudget\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C730CF91-40C5-4824-90A6-A940BEC7D12E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78D49D96-2D8D-4C5A-B770-FFCB502E037A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6640" activeTab="3" xr2:uid="{5373AB19-D84C-490D-97DC-C516D358024A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6640" xr2:uid="{5373AB19-D84C-490D-97DC-C516D358024A}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe-Directions" sheetId="6" r:id="rId1"/>
     <sheet name="Master" sheetId="5" r:id="rId2"/>
-    <sheet name="9.0-Trade" sheetId="12" r:id="rId3"/>
-    <sheet name="9.0-LawOfRiver" sheetId="13" r:id="rId4"/>
-    <sheet name="9.0-PlotUse" sheetId="14" r:id="rId5"/>
-    <sheet name="9.0-PlotStorage" sheetId="15" r:id="rId6"/>
+    <sheet name="11.0-Trade" sheetId="12" r:id="rId3"/>
+    <sheet name="11.0-LawOfRiver" sheetId="13" r:id="rId4"/>
+    <sheet name="11.0-PlotUse" sheetId="14" r:id="rId5"/>
+    <sheet name="11.0-PlotStorage" sheetId="15" r:id="rId6"/>
     <sheet name="Millenium-LawOfRiver" sheetId="11" r:id="rId7"/>
     <sheet name="HydrologicScenarios" sheetId="7" r:id="rId8"/>
     <sheet name="Powell-Elevation-Area" sheetId="2" r:id="rId9"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="168">
   <si>
     <t xml:space="preserve">    To Upper Basin</t>
   </si>
@@ -513,25 +513,31 @@
     <t>A completed role play of the Millennium Drought continuing for 10 more years following the Law of the River for all political decisions</t>
   </si>
   <si>
-    <t>9.0-LawOfRiver</t>
+    <t>4.9 to 6.5 feet per year for Powell, 5.5 to 6.4 feet per year from Schmidt et al (2016); 5.7 to 6.8 in Moreo (2015)</t>
   </si>
   <si>
-    <t>A completed role play with Lee Ferry natural flow of 9.0 maf per year for 5 years following the Law of the River for all political decisions</t>
+    <t>11.0-Trade</t>
   </si>
   <si>
-    <t>9.0-Trade</t>
+    <t>11.0-LawOfRiver</t>
   </si>
   <si>
-    <t>A completed role play with Lee Ferry natural flow of 9.0 maf per year for 5 years allowing trades between users. Trades in Years 1 and 2 earn the Upper Basin $0.75 Billion and get the Upper Basin on a path of conservation and softer landing for this severe event.</t>
+    <t>11.0-PlotUse</t>
   </si>
   <si>
-    <t>9.0-PlotUse</t>
+    <t>11.0-PlotStorage</t>
   </si>
   <si>
-    <t>Compare Upper Basin consumptive use for 9.0-Trade and 9.0-LawOfRiver</t>
+    <t>Compare Upper Basin storage account balance for 11.0-Trade and 11.0-LawOfRiver</t>
   </si>
   <si>
-    <t>4.9 to 6.5 feet per year for Powell, 5.5 to 6.4 feet per year from Schmidt et al (2016); 5.7 to 6.8 in Moreo (2015)</t>
+    <t>Compare Upper Basin consumptive use for 11.0-Trade and 11.0-LawOfRiver</t>
+  </si>
+  <si>
+    <t>A completed role play with Lee Ferry natural flow of 11.0 maf per year for 5 years following the Law of the River for all political decisions</t>
+  </si>
+  <si>
+    <t>A completed role play with Lee Ferry natural flow of 11.0 maf per year for 5 years allowing trades between users. Trades in Years 1 through 3 earn the Upper Basin $0.5 Billion and get the Upper Basin on a path of conservation and softer landing for this severe event.</t>
   </si>
 </sst>
 </file>
@@ -884,15 +890,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -906,6 +903,12 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -916,6 +919,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1907,7 +1913,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'9.0-LawOfRiver'!$C$21:$G$21</c:f>
+              <c:f>'11.0-LawOfRiver'!$C$21:$G$21</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -1930,7 +1936,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'9.0-LawOfRiver'!$C$49:$G$49</c:f>
+              <c:f>'11.0-LawOfRiver'!$C$49:$G$49</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1941,13 +1947,13 @@
                   <c:v>4.2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.7512385116186153</c:v>
+                  <c:v>3.3782273122835065</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.75</c:v>
+                  <c:v>2.4112853600768069</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.75</c:v>
+                  <c:v>2.4079688711010352</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1991,7 +1997,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'9.0-Trade'!$C$21:$G$21</c:f>
+              <c:f>'11.0-Trade'!$C$21:$G$21</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -2014,24 +2020,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'9.0-Trade'!$C$49:$G$49</c:f>
+              <c:f>'11.0-Trade'!$C$49:$G$49</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>3.5999999999999996</c:v>
+                  <c:v>3.8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.9</c:v>
+                  <c:v>3.3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>2.8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.5</c:v>
+                  <c:v>2.6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>2.6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2401,7 +2407,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'9.0-LawOfRiver'!$C$21:$G$21</c:f>
+              <c:f>'11.0-LawOfRiver'!$C$21:$G$21</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -2424,7 +2430,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'9.0-LawOfRiver'!$C$25:$G$25</c:f>
+              <c:f>'11.0-LawOfRiver'!$C$25:$G$25</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="5"/>
@@ -2432,16 +2438,16 @@
                   <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.017257133649303</c:v>
+                  <c:v>9.0172571336493021</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.1942915791521944</c:v>
+                  <c:v>7.1088601682676069</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>6.1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>6.1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2485,7 +2491,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'9.0-Trade'!$C$21:$G$21</c:f>
+              <c:f>'11.0-Trade'!$C$21:$G$21</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -2508,7 +2514,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'9.0-Trade'!$C$25:$G$25</c:f>
+              <c:f>'11.0-Trade'!$C$25:$G$25</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="5"/>
@@ -2516,16 +2522,16 @@
                   <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.9172571336493043</c:v>
+                  <c:v>8.9172571336493043</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.0044422142300484</c:v>
+                  <c:v>7.4184595445476385</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.5840169164901154</c:v>
+                  <c:v>6.4827904842124324</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.73776949495207056</c:v>
+                  <c:v>6.2890185479502954</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -21096,7 +21102,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{A297EC62-A5CD-4158-9592-AC76E370FCC0}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="63" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="76" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -21107,7 +21113,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{82902265-0E0F-4DE3-8482-388886F7C2EB}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="63" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="76" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -21118,7 +21124,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8668254" cy="6289524"/>
+    <xdr:ext cx="12996612" cy="9437270"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -21151,7 +21157,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8668254" cy="6289524"/>
+    <xdr:ext cx="12996612" cy="9437270"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -21639,10 +21645,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{447CC9A2-4C52-453A-A3CD-EA6E59E26162}">
-  <dimension ref="A1:L31"/>
+  <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -21682,20 +21688,20 @@
       <c r="D3"/>
     </row>
     <row r="4" spans="1:12" ht="164.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="52" t="s">
+      <c r="A4" s="62" t="s">
         <v>118</v>
       </c>
-      <c r="B4" s="52"/>
-      <c r="C4" s="52"/>
-      <c r="D4" s="52"/>
-      <c r="E4" s="52"/>
-      <c r="F4" s="52"/>
-      <c r="G4" s="52"/>
-      <c r="H4" s="52"/>
-      <c r="I4" s="52"/>
-      <c r="J4" s="52"/>
-      <c r="K4" s="52"/>
-      <c r="L4" s="52"/>
+      <c r="B4" s="62"/>
+      <c r="C4" s="62"/>
+      <c r="D4" s="62"/>
+      <c r="E4" s="62"/>
+      <c r="F4" s="62"/>
+      <c r="G4" s="62"/>
+      <c r="H4" s="62"/>
+      <c r="I4" s="62"/>
+      <c r="J4" s="62"/>
+      <c r="K4" s="62"/>
+      <c r="L4" s="62"/>
     </row>
     <row r="5" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="16"/>
@@ -21711,236 +21717,236 @@
       <c r="L5" s="16"/>
     </row>
     <row r="6" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="56" t="s">
+      <c r="A6" s="53" t="s">
         <v>123</v>
       </c>
-      <c r="B6" s="57"/>
-      <c r="C6" s="57"/>
-      <c r="D6" s="57"/>
-      <c r="E6" s="57"/>
-      <c r="F6" s="57"/>
-      <c r="G6" s="57"/>
-      <c r="H6" s="57"/>
-      <c r="I6" s="57"/>
-      <c r="J6" s="57"/>
-      <c r="K6" s="57"/>
-      <c r="L6" s="58"/>
+      <c r="B6" s="54"/>
+      <c r="C6" s="54"/>
+      <c r="D6" s="54"/>
+      <c r="E6" s="54"/>
+      <c r="F6" s="54"/>
+      <c r="G6" s="54"/>
+      <c r="H6" s="54"/>
+      <c r="I6" s="54"/>
+      <c r="J6" s="54"/>
+      <c r="K6" s="54"/>
+      <c r="L6" s="55"/>
     </row>
     <row r="7" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="29">
         <v>1</v>
       </c>
-      <c r="B7" s="53" t="s">
+      <c r="B7" s="56" t="s">
         <v>119</v>
       </c>
-      <c r="C7" s="53"/>
-      <c r="D7" s="53"/>
-      <c r="E7" s="53"/>
-      <c r="F7" s="53"/>
-      <c r="G7" s="53"/>
-      <c r="H7" s="53"/>
-      <c r="I7" s="53"/>
-      <c r="J7" s="53"/>
-      <c r="K7" s="53"/>
-      <c r="L7" s="54"/>
+      <c r="C7" s="56"/>
+      <c r="D7" s="56"/>
+      <c r="E7" s="56"/>
+      <c r="F7" s="56"/>
+      <c r="G7" s="56"/>
+      <c r="H7" s="56"/>
+      <c r="I7" s="56"/>
+      <c r="J7" s="56"/>
+      <c r="K7" s="56"/>
+      <c r="L7" s="57"/>
     </row>
     <row r="8" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="29">
         <v>2</v>
       </c>
-      <c r="B8" s="53" t="s">
+      <c r="B8" s="56" t="s">
         <v>99</v>
       </c>
-      <c r="C8" s="53"/>
-      <c r="D8" s="53"/>
-      <c r="E8" s="53"/>
-      <c r="F8" s="53"/>
-      <c r="G8" s="53"/>
-      <c r="H8" s="53"/>
-      <c r="I8" s="53"/>
-      <c r="J8" s="53"/>
-      <c r="K8" s="53"/>
-      <c r="L8" s="54"/>
+      <c r="C8" s="56"/>
+      <c r="D8" s="56"/>
+      <c r="E8" s="56"/>
+      <c r="F8" s="56"/>
+      <c r="G8" s="56"/>
+      <c r="H8" s="56"/>
+      <c r="I8" s="56"/>
+      <c r="J8" s="56"/>
+      <c r="K8" s="56"/>
+      <c r="L8" s="57"/>
     </row>
     <row r="9" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="29">
         <v>3</v>
       </c>
-      <c r="B9" s="53" t="s">
+      <c r="B9" s="56" t="s">
         <v>55</v>
       </c>
-      <c r="C9" s="53"/>
-      <c r="D9" s="53"/>
-      <c r="E9" s="53"/>
-      <c r="F9" s="53"/>
-      <c r="G9" s="53"/>
-      <c r="H9" s="53"/>
-      <c r="I9" s="53"/>
-      <c r="J9" s="53"/>
-      <c r="K9" s="53"/>
-      <c r="L9" s="54"/>
+      <c r="C9" s="56"/>
+      <c r="D9" s="56"/>
+      <c r="E9" s="56"/>
+      <c r="F9" s="56"/>
+      <c r="G9" s="56"/>
+      <c r="H9" s="56"/>
+      <c r="I9" s="56"/>
+      <c r="J9" s="56"/>
+      <c r="K9" s="56"/>
+      <c r="L9" s="57"/>
     </row>
     <row r="10" spans="1:12" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="29">
         <v>4</v>
       </c>
-      <c r="B10" s="53" t="s">
+      <c r="B10" s="56" t="s">
         <v>100</v>
       </c>
-      <c r="C10" s="53"/>
-      <c r="D10" s="53"/>
-      <c r="E10" s="53"/>
-      <c r="F10" s="53"/>
-      <c r="G10" s="53"/>
-      <c r="H10" s="53"/>
-      <c r="I10" s="53"/>
-      <c r="J10" s="53"/>
-      <c r="K10" s="53"/>
-      <c r="L10" s="54"/>
+      <c r="C10" s="56"/>
+      <c r="D10" s="56"/>
+      <c r="E10" s="56"/>
+      <c r="F10" s="56"/>
+      <c r="G10" s="56"/>
+      <c r="H10" s="56"/>
+      <c r="I10" s="56"/>
+      <c r="J10" s="56"/>
+      <c r="K10" s="56"/>
+      <c r="L10" s="57"/>
     </row>
     <row r="11" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="29">
         <v>5</v>
       </c>
-      <c r="B11" s="53" t="s">
+      <c r="B11" s="56" t="s">
         <v>57</v>
       </c>
-      <c r="C11" s="53"/>
-      <c r="D11" s="53"/>
-      <c r="E11" s="53"/>
-      <c r="F11" s="53"/>
-      <c r="G11" s="53"/>
-      <c r="H11" s="53"/>
-      <c r="I11" s="53"/>
-      <c r="J11" s="53"/>
-      <c r="K11" s="53"/>
-      <c r="L11" s="54"/>
+      <c r="C11" s="56"/>
+      <c r="D11" s="56"/>
+      <c r="E11" s="56"/>
+      <c r="F11" s="56"/>
+      <c r="G11" s="56"/>
+      <c r="H11" s="56"/>
+      <c r="I11" s="56"/>
+      <c r="J11" s="56"/>
+      <c r="K11" s="56"/>
+      <c r="L11" s="57"/>
     </row>
     <row r="12" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="29">
         <v>6</v>
       </c>
-      <c r="B12" s="53" t="s">
+      <c r="B12" s="56" t="s">
         <v>58</v>
       </c>
-      <c r="C12" s="53"/>
-      <c r="D12" s="53"/>
-      <c r="E12" s="53"/>
-      <c r="F12" s="53"/>
-      <c r="G12" s="53"/>
-      <c r="H12" s="53"/>
-      <c r="I12" s="53"/>
-      <c r="J12" s="53"/>
-      <c r="K12" s="53"/>
-      <c r="L12" s="54"/>
+      <c r="C12" s="56"/>
+      <c r="D12" s="56"/>
+      <c r="E12" s="56"/>
+      <c r="F12" s="56"/>
+      <c r="G12" s="56"/>
+      <c r="H12" s="56"/>
+      <c r="I12" s="56"/>
+      <c r="J12" s="56"/>
+      <c r="K12" s="56"/>
+      <c r="L12" s="57"/>
     </row>
     <row r="13" spans="1:12" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="29">
         <v>7</v>
       </c>
-      <c r="B13" s="53" t="s">
+      <c r="B13" s="56" t="s">
         <v>120</v>
       </c>
-      <c r="C13" s="53"/>
-      <c r="D13" s="53"/>
-      <c r="E13" s="53"/>
-      <c r="F13" s="53"/>
-      <c r="G13" s="53"/>
-      <c r="H13" s="53"/>
-      <c r="I13" s="53"/>
-      <c r="J13" s="53"/>
-      <c r="K13" s="53"/>
-      <c r="L13" s="54"/>
+      <c r="C13" s="56"/>
+      <c r="D13" s="56"/>
+      <c r="E13" s="56"/>
+      <c r="F13" s="56"/>
+      <c r="G13" s="56"/>
+      <c r="H13" s="56"/>
+      <c r="I13" s="56"/>
+      <c r="J13" s="56"/>
+      <c r="K13" s="56"/>
+      <c r="L13" s="57"/>
     </row>
     <row r="14" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="29">
         <v>8</v>
       </c>
-      <c r="B14" s="53" t="s">
+      <c r="B14" s="56" t="s">
         <v>121</v>
       </c>
-      <c r="C14" s="53"/>
-      <c r="D14" s="53"/>
-      <c r="E14" s="53"/>
-      <c r="F14" s="53"/>
-      <c r="G14" s="53"/>
-      <c r="H14" s="53"/>
-      <c r="I14" s="53"/>
-      <c r="J14" s="53"/>
-      <c r="K14" s="53"/>
-      <c r="L14" s="54"/>
+      <c r="C14" s="56"/>
+      <c r="D14" s="56"/>
+      <c r="E14" s="56"/>
+      <c r="F14" s="56"/>
+      <c r="G14" s="56"/>
+      <c r="H14" s="56"/>
+      <c r="I14" s="56"/>
+      <c r="J14" s="56"/>
+      <c r="K14" s="56"/>
+      <c r="L14" s="57"/>
     </row>
     <row r="15" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="29">
         <v>9</v>
       </c>
-      <c r="B15" s="53" t="s">
+      <c r="B15" s="56" t="s">
         <v>122</v>
       </c>
-      <c r="C15" s="53"/>
-      <c r="D15" s="53"/>
-      <c r="E15" s="53"/>
-      <c r="F15" s="53"/>
-      <c r="G15" s="53"/>
-      <c r="H15" s="53"/>
-      <c r="I15" s="53"/>
-      <c r="J15" s="53"/>
-      <c r="K15" s="53"/>
-      <c r="L15" s="54"/>
+      <c r="C15" s="56"/>
+      <c r="D15" s="56"/>
+      <c r="E15" s="56"/>
+      <c r="F15" s="56"/>
+      <c r="G15" s="56"/>
+      <c r="H15" s="56"/>
+      <c r="I15" s="56"/>
+      <c r="J15" s="56"/>
+      <c r="K15" s="56"/>
+      <c r="L15" s="57"/>
     </row>
     <row r="16" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="29">
         <v>10</v>
       </c>
-      <c r="B16" s="53" t="s">
+      <c r="B16" s="56" t="s">
         <v>59</v>
       </c>
-      <c r="C16" s="53"/>
-      <c r="D16" s="53"/>
-      <c r="E16" s="53"/>
-      <c r="F16" s="53"/>
-      <c r="G16" s="53"/>
-      <c r="H16" s="53"/>
-      <c r="I16" s="53"/>
-      <c r="J16" s="53"/>
-      <c r="K16" s="53"/>
-      <c r="L16" s="54"/>
+      <c r="C16" s="56"/>
+      <c r="D16" s="56"/>
+      <c r="E16" s="56"/>
+      <c r="F16" s="56"/>
+      <c r="G16" s="56"/>
+      <c r="H16" s="56"/>
+      <c r="I16" s="56"/>
+      <c r="J16" s="56"/>
+      <c r="K16" s="56"/>
+      <c r="L16" s="57"/>
     </row>
     <row r="17" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="29">
         <v>11</v>
       </c>
-      <c r="B17" s="59" t="s">
+      <c r="B17" s="58" t="s">
         <v>60</v>
       </c>
-      <c r="C17" s="59"/>
-      <c r="D17" s="59"/>
-      <c r="E17" s="59"/>
-      <c r="F17" s="59"/>
-      <c r="G17" s="59"/>
-      <c r="H17" s="59"/>
-      <c r="I17" s="59"/>
-      <c r="J17" s="59"/>
-      <c r="K17" s="59"/>
-      <c r="L17" s="60"/>
+      <c r="C17" s="58"/>
+      <c r="D17" s="58"/>
+      <c r="E17" s="58"/>
+      <c r="F17" s="58"/>
+      <c r="G17" s="58"/>
+      <c r="H17" s="58"/>
+      <c r="I17" s="58"/>
+      <c r="J17" s="58"/>
+      <c r="K17" s="58"/>
+      <c r="L17" s="59"/>
     </row>
     <row r="18" spans="1:12" ht="32" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="29">
         <v>12</v>
       </c>
-      <c r="B18" s="61" t="s">
+      <c r="B18" s="60" t="s">
         <v>108</v>
       </c>
-      <c r="C18" s="61"/>
-      <c r="D18" s="61"/>
-      <c r="E18" s="61"/>
-      <c r="F18" s="61"/>
-      <c r="G18" s="61"/>
-      <c r="H18" s="61"/>
-      <c r="I18" s="61"/>
-      <c r="J18" s="61"/>
-      <c r="K18" s="61"/>
-      <c r="L18" s="62"/>
+      <c r="C18" s="60"/>
+      <c r="D18" s="60"/>
+      <c r="E18" s="60"/>
+      <c r="F18" s="60"/>
+      <c r="G18" s="60"/>
+      <c r="H18" s="60"/>
+      <c r="I18" s="60"/>
+      <c r="J18" s="60"/>
+      <c r="K18" s="60"/>
+      <c r="L18" s="61"/>
     </row>
     <row r="19" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B19" s="27"/>
@@ -21970,76 +21976,89 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B22" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C22" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B23" s="2" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="C23" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B24" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C24" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B25" s="2" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="C25" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B26" s="2" t="s">
-        <v>104</v>
+        <v>157</v>
       </c>
       <c r="C26" t="s">
-        <v>105</v>
+        <v>158</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B27" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C27" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B28" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C28" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A30" s="1" t="s">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A31" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="55" t="s">
+    <row r="32" spans="1:12" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="52" t="s">
         <v>124</v>
       </c>
-      <c r="B31" s="55"/>
-      <c r="C31" s="55"/>
-      <c r="D31" s="55"/>
-      <c r="E31" s="55"/>
-      <c r="F31" s="55"/>
-      <c r="G31" s="55"/>
-      <c r="H31" s="55"/>
-      <c r="I31" s="55"/>
-      <c r="J31" s="55"/>
-      <c r="K31" s="55"/>
-      <c r="L31" s="55"/>
+      <c r="B32" s="52"/>
+      <c r="C32" s="52"/>
+      <c r="D32" s="52"/>
+      <c r="E32" s="52"/>
+      <c r="F32" s="52"/>
+      <c r="G32" s="52"/>
+      <c r="H32" s="52"/>
+      <c r="I32" s="52"/>
+      <c r="J32" s="52"/>
+      <c r="K32" s="52"/>
+      <c r="L32" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A31:L31"/>
+    <mergeCell ref="A4:L4"/>
+    <mergeCell ref="B9:L9"/>
+    <mergeCell ref="B11:L11"/>
+    <mergeCell ref="B12:L12"/>
+    <mergeCell ref="B13:L13"/>
+    <mergeCell ref="A32:L32"/>
     <mergeCell ref="A6:L6"/>
     <mergeCell ref="B10:L10"/>
     <mergeCell ref="B7:L7"/>
@@ -22049,11 +22068,6 @@
     <mergeCell ref="B16:L16"/>
     <mergeCell ref="B17:L17"/>
     <mergeCell ref="B18:L18"/>
-    <mergeCell ref="A4:L4"/>
-    <mergeCell ref="B9:L9"/>
-    <mergeCell ref="B11:L11"/>
-    <mergeCell ref="B12:L12"/>
-    <mergeCell ref="B13:L13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -22063,7 +22077,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3356767-5983-45FB-80E4-1C5DE08E38A0}">
   <dimension ref="A1:R62"/>
   <sheetViews>
-    <sheetView topLeftCell="A45" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView topLeftCell="A26" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="C49" sqref="C49:G52"/>
     </sheetView>
   </sheetViews>
@@ -23982,8 +23996,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{710BD1F0-C024-4B0C-A52B-7568661161E6}">
   <dimension ref="A1:R62"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49:D49"/>
+    <sheetView topLeftCell="A37" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -24209,43 +24223,43 @@
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="12">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D22" s="12">
         <f>C22</f>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E22" s="12">
         <f t="shared" ref="E22:G22" si="0">D22</f>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F22" s="12">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G22" s="12">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="H22" s="12">
         <f t="shared" ref="H22:L22" si="1">G22</f>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I22" s="12">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="J22" s="12">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="K22" s="12">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="L22" s="12">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.35">
@@ -24305,39 +24319,39 @@
       </c>
       <c r="D24" s="15">
         <f>IF(D$22&lt;&gt;"",C57,"")</f>
-        <v>17.311102320000032</v>
+        <v>19.111102320000029</v>
       </c>
       <c r="E24" s="15">
         <f t="shared" ref="E24:L24" si="3">IF(E$22&lt;&gt;"",D57,"")</f>
-        <v>14.336123034000025</v>
+        <v>17.682257605000633</v>
       </c>
       <c r="F24" s="15">
         <f t="shared" si="3"/>
-        <v>12.355914503999429</v>
+        <v>16.795996721501201</v>
       </c>
       <c r="G24" s="15">
         <f t="shared" si="3"/>
-        <v>10.938149218998831</v>
+        <v>16.138332072001205</v>
       </c>
       <c r="H24" s="15">
         <f t="shared" si="3"/>
-        <v>10.067667593999406</v>
+        <v>15.500628101901777</v>
       </c>
       <c r="I24" s="15">
         <f t="shared" si="3"/>
-        <v>8.2252786064993764</v>
+        <v>15.484011271901204</v>
       </c>
       <c r="J24" s="15">
         <f t="shared" si="3"/>
-        <v>6.4458632384993759</v>
+        <v>15.46739444190063</v>
       </c>
       <c r="K24" s="15">
         <f t="shared" si="3"/>
-        <v>4.7288440154999769</v>
+        <v>15.450777611900055</v>
       </c>
       <c r="L24" s="15">
         <f t="shared" si="3"/>
-        <v>3.0730837079994062</v>
+        <v>15.435417829300054</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.35">
@@ -24350,39 +24364,39 @@
       </c>
       <c r="D25" s="15">
         <f>IF(D22&lt;&gt;"",C54,"")</f>
-        <v>6.9172571336493043</v>
+        <v>8.9172571336493043</v>
       </c>
       <c r="E25" s="15">
         <f t="shared" ref="E25:L27" si="4">IF(E22&lt;&gt;"",D54,"")</f>
-        <v>3.0044422142300484</v>
+        <v>7.4184595445476385</v>
       </c>
       <c r="F25" s="15">
         <f t="shared" si="4"/>
-        <v>1.5840169164901154</v>
+        <v>6.4827904842124324</v>
       </c>
       <c r="G25" s="15">
         <f t="shared" si="4"/>
-        <v>0.73776949495207056</v>
+        <v>6.2890185479502954</v>
       </c>
       <c r="H25" s="15">
         <f t="shared" si="4"/>
-        <v>0.44032021694419621</v>
+        <v>6.0997100374240141</v>
       </c>
       <c r="I25" s="15">
         <f t="shared" si="4"/>
-        <v>-0.83921864324572337</v>
+        <v>6.5153741465265966</v>
       </c>
       <c r="J25" s="15">
         <f t="shared" si="4"/>
-        <v>-2.026734389663154</v>
+        <v>6.9078717247423267</v>
       </c>
       <c r="K25" s="15">
         <f t="shared" si="4"/>
-        <v>-3.1037951210217347</v>
+        <v>7.2784255226769599</v>
       </c>
       <c r="L25" s="15">
         <f t="shared" si="4"/>
-        <v>-4.0329953964385226</v>
+        <v>7.6287871582406748</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.35">
@@ -24395,39 +24409,39 @@
       </c>
       <c r="D26" s="15">
         <f>IF(D23&lt;&gt;"",C55,"")</f>
-        <v>10.393845186350726</v>
+        <v>10.193845186350726</v>
       </c>
       <c r="E26" s="15">
         <f t="shared" si="4"/>
-        <v>11.331680819769977</v>
+        <v>10.263798060452993</v>
       </c>
       <c r="F26" s="15">
         <f t="shared" si="4"/>
-        <v>10.771897587509313</v>
+        <v>10.313206237288769</v>
       </c>
       <c r="G26" s="15">
         <f t="shared" si="4"/>
-        <v>10.20037972404676</v>
+        <v>9.849313524050908</v>
       </c>
       <c r="H26" s="15">
         <f t="shared" si="4"/>
-        <v>9.6273473770552105</v>
+        <v>9.4009180644777626</v>
       </c>
       <c r="I26" s="15">
         <f t="shared" si="4"/>
-        <v>9.0644972497451004</v>
+        <v>8.9686371253746078</v>
       </c>
       <c r="J26" s="15">
         <f t="shared" si="4"/>
-        <v>8.4725976281625304</v>
+        <v>8.5595227171583037</v>
       </c>
       <c r="K26" s="15">
         <f t="shared" si="4"/>
-        <v>7.8326391365217116</v>
+        <v>8.1723520892230948</v>
       </c>
       <c r="L26" s="15">
         <f t="shared" si="4"/>
-        <v>7.1060791044379288</v>
+        <v>7.8066306710593789</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.35">
@@ -24494,39 +24508,39 @@
       </c>
       <c r="D29" s="15">
         <f t="shared" ref="D29:L30" si="5">IF(D22&lt;&gt;"",$B29*D$24,"")</f>
-        <v>8.6555511600000159</v>
+        <v>9.5555511600000145</v>
       </c>
       <c r="E29" s="15">
         <f t="shared" si="5"/>
-        <v>7.1680615170000124</v>
+        <v>8.8411288025003163</v>
       </c>
       <c r="F29" s="15">
         <f t="shared" si="5"/>
-        <v>6.1779572519997146</v>
+        <v>8.3979983607506004</v>
       </c>
       <c r="G29" s="15">
         <f t="shared" si="5"/>
-        <v>5.4690746094994154</v>
+        <v>8.0691660360006026</v>
       </c>
       <c r="H29" s="15">
         <f t="shared" si="5"/>
-        <v>5.0338337969997031</v>
+        <v>7.7503140509508883</v>
       </c>
       <c r="I29" s="15">
         <f t="shared" si="5"/>
-        <v>4.1126393032496882</v>
+        <v>7.7420056359506022</v>
       </c>
       <c r="J29" s="15">
         <f t="shared" si="5"/>
-        <v>3.222931619249688</v>
+        <v>7.7336972209503152</v>
       </c>
       <c r="K29" s="15">
         <f t="shared" si="5"/>
-        <v>2.3644220077499885</v>
+        <v>7.7253888059500273</v>
       </c>
       <c r="L29" s="15">
         <f t="shared" si="5"/>
-        <v>1.5365418539997031</v>
+        <v>7.7177089146500268</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.35">
@@ -24543,39 +24557,39 @@
       </c>
       <c r="D30" s="15">
         <f t="shared" si="5"/>
-        <v>8.6555511600000159</v>
+        <v>9.5555511600000145</v>
       </c>
       <c r="E30" s="15">
         <f t="shared" si="5"/>
-        <v>7.1680615170000124</v>
+        <v>8.8411288025003163</v>
       </c>
       <c r="F30" s="15">
         <f t="shared" si="5"/>
-        <v>6.1779572519997146</v>
+        <v>8.3979983607506004</v>
       </c>
       <c r="G30" s="15">
         <f t="shared" si="5"/>
-        <v>5.4690746094994154</v>
+        <v>8.0691660360006026</v>
       </c>
       <c r="H30" s="15">
         <f t="shared" si="5"/>
-        <v>5.0338337969997031</v>
+        <v>7.7503140509508883</v>
       </c>
       <c r="I30" s="15">
         <f t="shared" si="5"/>
-        <v>4.1126393032496882</v>
+        <v>7.7420056359506022</v>
       </c>
       <c r="J30" s="15">
         <f t="shared" si="5"/>
-        <v>3.222931619249688</v>
+        <v>7.7336972209503152</v>
       </c>
       <c r="K30" s="15">
         <f t="shared" si="5"/>
-        <v>2.3644220077499885</v>
+        <v>7.7253888059500273</v>
       </c>
       <c r="L30" s="15">
         <f t="shared" si="5"/>
-        <v>1.5365418539997031</v>
+        <v>7.7177089146500268</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.35">
@@ -24589,39 +24603,39 @@
       </c>
       <c r="D31" s="15">
         <f>IF(D$22&lt;&gt;"",VLOOKUP(D29*1000000,'Powell-Elevation-Area'!$B$5:$D$689,3)*$B$18/1000000 + VLOOKUP(D30*1000000,'Mead-Elevation-Area'!$B$5:$D$676,3)*$C$18/1000000,"")</f>
-        <v>0.907979286</v>
+        <v>0.96184471499940005</v>
       </c>
       <c r="E31" s="15">
         <f>IF(E$22&lt;&gt;"",VLOOKUP(E29*1000000,'Powell-Elevation-Area'!$B$5:$D$689,3)*$B$18/1000000 + VLOOKUP(E30*1000000,'Mead-Elevation-Area'!$B$5:$D$676,3)*$C$18/1000000,"")</f>
-        <v>0.81320853000060001</v>
+        <v>0.91926088349942692</v>
       </c>
       <c r="F31" s="15">
         <f>IF(F$22&lt;&gt;"",VLOOKUP(F29*1000000,'Powell-Elevation-Area'!$B$5:$D$689,3)*$B$18/1000000 + VLOOKUP(F30*1000000,'Mead-Elevation-Area'!$B$5:$D$676,3)*$C$18/1000000,"")</f>
-        <v>0.75076528500060002</v>
+        <v>0.89066464949999991</v>
       </c>
       <c r="G31" s="15">
         <f>IF(G$22&lt;&gt;"",VLOOKUP(G29*1000000,'Powell-Elevation-Area'!$B$5:$D$689,3)*$B$18/1000000 + VLOOKUP(G30*1000000,'Mead-Elevation-Area'!$B$5:$D$676,3)*$C$18/1000000,"")</f>
-        <v>0.70348162499942701</v>
+        <v>0.87070397009942702</v>
       </c>
       <c r="H31" s="15">
         <f>IF(H$22&lt;&gt;"",VLOOKUP(H29*1000000,'Powell-Elevation-Area'!$B$5:$D$689,3)*$B$18/1000000 + VLOOKUP(H30*1000000,'Mead-Elevation-Area'!$B$5:$D$676,3)*$C$18/1000000,"")</f>
-        <v>0.67538898750002696</v>
+        <v>0.84961683000057309</v>
       </c>
       <c r="I31" s="15">
         <f>IF(I$22&lt;&gt;"",VLOOKUP(I29*1000000,'Powell-Elevation-Area'!$B$5:$D$689,3)*$B$18/1000000 + VLOOKUP(I30*1000000,'Mead-Elevation-Area'!$B$5:$D$676,3)*$C$18/1000000,"")</f>
-        <v>0.61241536799999996</v>
+        <v>0.84961683000057309</v>
       </c>
       <c r="J31" s="15">
         <f>IF(J$22&lt;&gt;"",VLOOKUP(J29*1000000,'Powell-Elevation-Area'!$B$5:$D$689,3)*$B$18/1000000 + VLOOKUP(J30*1000000,'Mead-Elevation-Area'!$B$5:$D$676,3)*$C$18/1000000,"")</f>
-        <v>0.55001922299939998</v>
+        <v>0.84961683000057309</v>
       </c>
       <c r="K31" s="15">
         <f>IF(K$22&lt;&gt;"",VLOOKUP(K29*1000000,'Powell-Elevation-Area'!$B$5:$D$689,3)*$B$18/1000000 + VLOOKUP(K30*1000000,'Mead-Elevation-Area'!$B$5:$D$676,3)*$C$18/1000000,"")</f>
-        <v>0.48876030750057303</v>
+        <v>0.8483597826</v>
       </c>
       <c r="L31" s="15">
         <f>IF(L$22&lt;&gt;"",VLOOKUP(L29*1000000,'Powell-Elevation-Area'!$B$5:$D$689,3)*$B$18/1000000 + VLOOKUP(L30*1000000,'Mead-Elevation-Area'!$B$5:$D$676,3)*$C$18/1000000,"")</f>
-        <v>0.42522618899942699</v>
+        <v>0.84724978260060002</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.35">
@@ -24635,39 +24649,39 @@
       </c>
       <c r="D32" s="15">
         <f t="shared" ref="D32:L34" si="6">IF(D$22&lt;&gt;"",D$31*D25/D$24,"")</f>
-        <v>0.3628149194192557</v>
+        <v>0.44879758910166673</v>
       </c>
       <c r="E32" s="15">
         <f t="shared" si="6"/>
-        <v>0.17042529773993298</v>
+        <v>0.38566906033520454</v>
       </c>
       <c r="F32" s="15">
         <f t="shared" si="6"/>
-        <v>9.6247421538044664E-2</v>
+        <v>0.3437719362621387</v>
       </c>
       <c r="G32" s="15">
         <f t="shared" si="6"/>
-        <v>4.7449278007874338E-2</v>
+        <v>0.33930851052628203</v>
       </c>
       <c r="H32" s="15">
         <f t="shared" si="6"/>
-        <v>2.9538860189919618E-2</v>
+        <v>0.334335890897417</v>
       </c>
       <c r="I32" s="15">
         <f t="shared" si="6"/>
-        <v>-6.2484253582569434E-2</v>
+        <v>0.35750242178427005</v>
       </c>
       <c r="J32" s="15">
         <f t="shared" si="6"/>
-        <v>-0.17293926864141906</v>
+        <v>0.37944620206536739</v>
       </c>
       <c r="K32" s="15">
         <f t="shared" si="6"/>
-        <v>-0.32079972458321171</v>
+        <v>0.39963836443628564</v>
       </c>
       <c r="L32" s="15">
         <f t="shared" si="6"/>
-        <v>-0.55805029268018802</v>
+        <v>0.41874397783106587</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.35">
@@ -24681,39 +24695,39 @@
       </c>
       <c r="D33" s="15">
         <f t="shared" si="6"/>
-        <v>0.5451643665807443</v>
+        <v>0.51304712589773338</v>
       </c>
       <c r="E33" s="15">
         <f t="shared" si="6"/>
-        <v>0.64278323226066714</v>
+        <v>0.53359182316422227</v>
       </c>
       <c r="F33" s="15">
         <f t="shared" si="6"/>
-        <v>0.65451786346255536</v>
+        <v>0.54689271323786126</v>
       </c>
       <c r="G33" s="15">
         <f t="shared" si="6"/>
-        <v>0.65603234699155266</v>
+        <v>0.53139545957314493</v>
       </c>
       <c r="H33" s="15">
         <f t="shared" si="6"/>
-        <v>0.64585012731010738</v>
+        <v>0.51528093910315609</v>
       </c>
       <c r="I33" s="15">
         <f t="shared" si="6"/>
-        <v>0.67489962158256944</v>
+        <v>0.49211440821630298</v>
       </c>
       <c r="J33" s="15">
         <f t="shared" si="6"/>
-        <v>0.72295849164081905</v>
+        <v>0.47017062793520575</v>
       </c>
       <c r="K33" s="15">
         <f t="shared" si="6"/>
-        <v>0.80956003208378469</v>
+        <v>0.44872141816371436</v>
       </c>
       <c r="L33" s="15">
         <f t="shared" si="6"/>
-        <v>0.98327648167961512</v>
+        <v>0.42850580476953415</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.35">
@@ -24815,43 +24829,43 @@
       <c r="B36" s="1"/>
       <c r="C36" s="15">
         <f>IF(C$22&lt;&gt;"",C22-C35/2,"")</f>
-        <v>8.25</v>
+        <v>10.25</v>
       </c>
       <c r="D36" s="15">
         <f t="shared" ref="D36:L36" si="8">IF(D$22&lt;&gt;"",D22-D35/2,"")</f>
-        <v>8.25</v>
+        <v>10.25</v>
       </c>
       <c r="E36" s="15">
         <f t="shared" si="8"/>
-        <v>8.25</v>
+        <v>10.25</v>
       </c>
       <c r="F36" s="15">
         <f t="shared" si="8"/>
-        <v>8.25</v>
+        <v>10.25</v>
       </c>
       <c r="G36" s="15">
         <f t="shared" si="8"/>
-        <v>8.25</v>
+        <v>10.25</v>
       </c>
       <c r="H36" s="15">
         <f t="shared" si="8"/>
-        <v>8.25</v>
+        <v>10.25</v>
       </c>
       <c r="I36" s="15">
         <f t="shared" si="8"/>
-        <v>8.25</v>
+        <v>10.25</v>
       </c>
       <c r="J36" s="15">
         <f t="shared" si="8"/>
-        <v>8.25</v>
+        <v>10.25</v>
       </c>
       <c r="K36" s="15">
         <f t="shared" si="8"/>
-        <v>8.25</v>
+        <v>10.25</v>
       </c>
       <c r="L36" s="15">
         <f t="shared" si="8"/>
-        <v>8.25</v>
+        <v>10.25</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.35">
@@ -24861,43 +24875,43 @@
       <c r="B37" s="25"/>
       <c r="C37" s="15">
         <f>IF(C22&lt;&gt;"",MAX(0,C36-C38),"")</f>
-        <v>0.75</v>
+        <v>2.75</v>
       </c>
       <c r="D37" s="15">
         <f t="shared" ref="D37:L37" si="9">IF(D22&lt;&gt;"",MAX(0,D36-D38),"")</f>
-        <v>0.75</v>
+        <v>2.75</v>
       </c>
       <c r="E37" s="15">
         <f t="shared" si="9"/>
-        <v>0.75</v>
+        <v>2.75</v>
       </c>
       <c r="F37" s="15">
         <f t="shared" si="9"/>
-        <v>0.75</v>
+        <v>2.75</v>
       </c>
       <c r="G37" s="15">
         <f t="shared" si="9"/>
-        <v>0.75</v>
+        <v>2.75</v>
       </c>
       <c r="H37" s="15">
         <f t="shared" si="9"/>
-        <v>0.75</v>
+        <v>2.75</v>
       </c>
       <c r="I37" s="15">
         <f t="shared" si="9"/>
-        <v>0.75</v>
+        <v>2.75</v>
       </c>
       <c r="J37" s="15">
         <f t="shared" si="9"/>
-        <v>0.75</v>
+        <v>2.75</v>
       </c>
       <c r="K37" s="15">
         <f t="shared" si="9"/>
-        <v>0.75</v>
+        <v>2.75</v>
       </c>
       <c r="L37" s="15">
         <f t="shared" si="9"/>
-        <v>0.75</v>
+        <v>2.75</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.35">
@@ -24960,12 +24974,14 @@
       </c>
       <c r="B40" s="1"/>
       <c r="C40" s="26">
-        <v>0.7</v>
+        <v>0.5</v>
       </c>
       <c r="D40" s="26">
-        <v>1.4</v>
-      </c>
-      <c r="E40" s="26"/>
+        <v>0.5</v>
+      </c>
+      <c r="E40" s="26">
+        <v>0.5</v>
+      </c>
       <c r="F40" s="26"/>
       <c r="G40" s="26"/>
       <c r="H40" s="26"/>
@@ -24981,15 +24997,15 @@
       <c r="B41" s="1"/>
       <c r="C41" s="32">
         <f>350*C40</f>
-        <v>244.99999999999997</v>
+        <v>175</v>
       </c>
       <c r="D41" s="32">
         <f>350*D40</f>
-        <v>489.99999999999994</v>
+        <v>175</v>
       </c>
       <c r="E41" s="32">
         <f t="shared" ref="E41:G41" si="11">350*E40</f>
-        <v>0</v>
+        <v>175</v>
       </c>
       <c r="F41" s="32">
         <f t="shared" si="11"/>
@@ -25006,7 +25022,7 @@
       <c r="L41" s="32"/>
       <c r="M41" s="34">
         <f>SUM(C41:L41)</f>
-        <v>734.99999999999989</v>
+        <v>525</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.35">
@@ -25059,43 +25075,43 @@
       </c>
       <c r="C45" s="15">
         <f>IF(C$22&lt;&gt;"",C25+C37-C32-C40,"")</f>
-        <v>10.517257133649304</v>
+        <v>12.717257133649303</v>
       </c>
       <c r="D45" s="15">
         <f t="shared" ref="D45:L45" si="12">IF(D$22&lt;&gt;"",D25+D37-D32-D40,"")</f>
-        <v>5.9044422142300483</v>
+        <v>10.718459544547638</v>
       </c>
       <c r="E45" s="15">
         <f t="shared" si="12"/>
-        <v>3.5840169164901154</v>
+        <v>9.2827904842124322</v>
       </c>
       <c r="F45" s="15">
         <f>IF(F$22&lt;&gt;"",F25+F37-F32-F40,"")</f>
-        <v>2.2377694949520706</v>
+        <v>8.889018547950295</v>
       </c>
       <c r="G45" s="15">
         <f t="shared" si="12"/>
-        <v>1.4403202169441962</v>
+        <v>8.6997100374240137</v>
       </c>
       <c r="H45" s="15">
         <f t="shared" si="12"/>
-        <v>1.1607813567542766</v>
+        <v>8.5153741465265966</v>
       </c>
       <c r="I45" s="15">
         <f t="shared" si="12"/>
-        <v>-2.6734389663153939E-2</v>
+        <v>8.9078717247423267</v>
       </c>
       <c r="J45" s="15">
         <f t="shared" si="12"/>
-        <v>-1.1037951210217349</v>
+        <v>9.2784255226769599</v>
       </c>
       <c r="K45" s="15">
         <f t="shared" si="12"/>
-        <v>-2.032995396438523</v>
+        <v>9.6287871582406748</v>
       </c>
       <c r="L45" s="15">
         <f t="shared" si="12"/>
-        <v>-2.7249451037583343</v>
+        <v>9.9600431804096097</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.35">
@@ -25104,43 +25120,43 @@
       </c>
       <c r="C46" s="15">
         <f>IF(C$22&lt;&gt;"",C26+C38-C33+C40+C42+C23-C35/2,"")</f>
-        <v>17.860845186350726</v>
+        <v>17.660845186350727</v>
       </c>
       <c r="D46" s="15">
         <f t="shared" ref="D46:L46" si="13">IF(D$22&lt;&gt;"",D26+D38-D33+D40+D42+D23-D35/2,"")</f>
-        <v>18.798680819769977</v>
+        <v>17.730798060452994</v>
       </c>
       <c r="E46" s="15">
         <f t="shared" si="13"/>
-        <v>18.238897587509314</v>
+        <v>17.78020623728877</v>
       </c>
       <c r="F46" s="15">
         <f t="shared" si="13"/>
-        <v>17.667379724046761</v>
+        <v>17.316313524050909</v>
       </c>
       <c r="G46" s="15">
         <f t="shared" si="13"/>
-        <v>17.094347377055211</v>
+        <v>16.867918064477763</v>
       </c>
       <c r="H46" s="15">
         <f t="shared" si="13"/>
-        <v>16.531497249745101</v>
+        <v>16.435637125374608</v>
       </c>
       <c r="I46" s="15">
         <f t="shared" si="13"/>
-        <v>15.939597628162531</v>
+        <v>16.026522717158304</v>
       </c>
       <c r="J46" s="15">
         <f t="shared" si="13"/>
-        <v>15.299639136521712</v>
+        <v>15.639352089223095</v>
       </c>
       <c r="K46" s="15">
         <f t="shared" si="13"/>
-        <v>14.573079104437928</v>
+        <v>15.273630671059379</v>
       </c>
       <c r="L46" s="15">
         <f t="shared" si="13"/>
-        <v>13.672802622758313</v>
+        <v>14.928124866289846</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.35">
@@ -25209,21 +25225,19 @@
         <v>152</v>
       </c>
       <c r="C49" s="45">
-        <f>4.3-C40</f>
-        <v>3.5999999999999996</v>
+        <v>3.8</v>
       </c>
       <c r="D49" s="45">
-        <f>4.3-D40</f>
-        <v>2.9</v>
+        <v>3.3</v>
       </c>
       <c r="E49" s="45">
-        <v>2</v>
+        <v>2.8</v>
       </c>
       <c r="F49" s="45">
-        <v>1.5</v>
+        <v>2.6</v>
       </c>
       <c r="G49" s="45">
-        <v>1</v>
+        <v>2.6</v>
       </c>
       <c r="H49" s="26">
         <v>2</v>
@@ -25453,43 +25467,43 @@
       </c>
       <c r="C54" s="15">
         <f>IF(C$22&lt;&gt;"",C45-C49,"")</f>
-        <v>6.9172571336493043</v>
+        <v>8.9172571336493043</v>
       </c>
       <c r="D54" s="15">
         <f t="shared" ref="D54:L54" si="18">IF(D$22&lt;&gt;"",D45-D49,"")</f>
-        <v>3.0044422142300484</v>
+        <v>7.4184595445476385</v>
       </c>
       <c r="E54" s="15">
         <f t="shared" si="18"/>
-        <v>1.5840169164901154</v>
+        <v>6.4827904842124324</v>
       </c>
       <c r="F54" s="15">
         <f t="shared" si="18"/>
-        <v>0.73776949495207056</v>
+        <v>6.2890185479502954</v>
       </c>
       <c r="G54" s="15">
         <f t="shared" si="18"/>
-        <v>0.44032021694419621</v>
+        <v>6.0997100374240141</v>
       </c>
       <c r="H54" s="15">
         <f t="shared" si="18"/>
-        <v>-0.83921864324572337</v>
+        <v>6.5153741465265966</v>
       </c>
       <c r="I54" s="15">
         <f t="shared" si="18"/>
-        <v>-2.026734389663154</v>
+        <v>6.9078717247423267</v>
       </c>
       <c r="J54" s="15">
         <f t="shared" si="18"/>
-        <v>-3.1037951210217347</v>
+        <v>7.2784255226769599</v>
       </c>
       <c r="K54" s="15">
         <f t="shared" si="18"/>
-        <v>-4.0329953964385226</v>
+        <v>7.6287871582406748</v>
       </c>
       <c r="L54" s="15">
         <f t="shared" si="18"/>
-        <v>-4.7249451037583343</v>
+        <v>7.9600431804096097</v>
       </c>
       <c r="N54" s="41">
         <v>1040</v>
@@ -25514,43 +25528,43 @@
       </c>
       <c r="C55" s="15">
         <f>IF(C$22&lt;&gt;"",C46-C50-C51,"")</f>
-        <v>10.393845186350726</v>
+        <v>10.193845186350726</v>
       </c>
       <c r="D55" s="15">
         <f t="shared" ref="D55:L55" si="19">IF(D$22&lt;&gt;"",D46-D50-D51,"")</f>
-        <v>11.331680819769977</v>
+        <v>10.263798060452993</v>
       </c>
       <c r="E55" s="15">
         <f t="shared" si="19"/>
-        <v>10.771897587509313</v>
+        <v>10.313206237288769</v>
       </c>
       <c r="F55" s="15">
         <f t="shared" si="19"/>
-        <v>10.20037972404676</v>
+        <v>9.849313524050908</v>
       </c>
       <c r="G55" s="15">
         <f t="shared" si="19"/>
-        <v>9.6273473770552105</v>
+        <v>9.4009180644777626</v>
       </c>
       <c r="H55" s="15">
         <f t="shared" si="19"/>
-        <v>9.0644972497451004</v>
+        <v>8.9686371253746078</v>
       </c>
       <c r="I55" s="15">
         <f t="shared" si="19"/>
-        <v>8.4725976281625304</v>
+        <v>8.5595227171583037</v>
       </c>
       <c r="J55" s="15">
         <f t="shared" si="19"/>
-        <v>7.8326391365217116</v>
+        <v>8.1723520892230948</v>
       </c>
       <c r="K55" s="15">
         <f t="shared" si="19"/>
-        <v>7.1060791044379288</v>
+        <v>7.8066306710593789</v>
       </c>
       <c r="L55" s="15">
         <f t="shared" si="19"/>
-        <v>6.2058026227583136</v>
+        <v>7.4611248662898451</v>
       </c>
       <c r="N55" s="41">
         <v>1045</v>
@@ -25637,43 +25651,43 @@
       <c r="B57" s="1"/>
       <c r="C57" s="15">
         <f>IF(C$22&lt;&gt;"",SUM(C54:C56),"")</f>
-        <v>17.311102320000032</v>
+        <v>19.111102320000029</v>
       </c>
       <c r="D57" s="15">
         <f t="shared" ref="D57:L57" si="21">IF(D$22&lt;&gt;"",SUM(D54:D56),"")</f>
-        <v>14.336123034000025</v>
+        <v>17.682257605000633</v>
       </c>
       <c r="E57" s="15">
         <f t="shared" si="21"/>
-        <v>12.355914503999429</v>
+        <v>16.795996721501201</v>
       </c>
       <c r="F57" s="15">
         <f t="shared" si="21"/>
-        <v>10.938149218998831</v>
+        <v>16.138332072001205</v>
       </c>
       <c r="G57" s="15">
         <f t="shared" si="21"/>
-        <v>10.067667593999406</v>
+        <v>15.500628101901777</v>
       </c>
       <c r="H57" s="15">
         <f t="shared" si="21"/>
-        <v>8.2252786064993764</v>
+        <v>15.484011271901204</v>
       </c>
       <c r="I57" s="15">
         <f t="shared" si="21"/>
-        <v>6.4458632384993759</v>
+        <v>15.46739444190063</v>
       </c>
       <c r="J57" s="15">
         <f t="shared" si="21"/>
-        <v>4.7288440154999769</v>
+        <v>15.450777611900055</v>
       </c>
       <c r="K57" s="15">
         <f t="shared" si="21"/>
-        <v>3.0730837079994062</v>
+        <v>15.435417829300054</v>
       </c>
       <c r="L57" s="15">
         <f t="shared" si="21"/>
-        <v>1.4808575189999793</v>
+        <v>15.421168046699455</v>
       </c>
       <c r="N57" s="41">
         <v>1075</v>
@@ -25974,8 +25988,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6E878AF-96FE-424D-B802-94EDCA32030C}">
   <dimension ref="A1:R62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView topLeftCell="A30" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="N48" sqref="N48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -26137,7 +26151,7 @@
         <v>6</v>
       </c>
       <c r="D18" s="24" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.35">
@@ -26201,43 +26215,43 @@
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="12">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D22" s="12">
         <f>C22</f>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E22" s="12">
         <f t="shared" ref="E22:G22" si="0">D22</f>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F22" s="12">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G22" s="12">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="H22" s="12">
         <f t="shared" ref="H22:L22" si="1">G22</f>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I22" s="12">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="J22" s="12">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="K22" s="12">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="L22" s="12">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.35">
@@ -26297,39 +26311,39 @@
       </c>
       <c r="D24" s="15">
         <f>IF(D$22&lt;&gt;"",C57,"")</f>
-        <v>16.71110232000003</v>
+        <v>18.71110232000003</v>
       </c>
       <c r="E24" s="15">
         <f t="shared" ref="E24:L24" si="3">IF(E$22&lt;&gt;"",D57,"")</f>
-        <v>12.455911190000005</v>
+        <v>16.392913683000028</v>
       </c>
       <c r="F24" s="15">
         <f t="shared" si="3"/>
-        <v>8.8688760708802157</v>
+        <v>15.05395331571655</v>
       </c>
       <c r="G24" s="15">
         <f t="shared" si="3"/>
-        <v>8.4017965217796444</v>
+        <v>14.723767238139169</v>
       </c>
       <c r="H24" s="15">
         <f t="shared" si="3"/>
-        <v>7.9494535507790722</v>
+        <v>14.407226771938737</v>
       </c>
       <c r="I24" s="15">
         <f t="shared" si="3"/>
-        <v>6.2627052151790732</v>
+        <v>14.508747251838164</v>
       </c>
       <c r="J24" s="15">
         <f t="shared" si="3"/>
-        <v>4.636290714178501</v>
+        <v>14.607996684339339</v>
       </c>
       <c r="K24" s="15">
         <f t="shared" si="3"/>
-        <v>3.0685236511785026</v>
+        <v>14.702710079338168</v>
       </c>
       <c r="L24" s="15">
         <f t="shared" si="3"/>
-        <v>1.5609641476779306</v>
+        <v>14.795152484238169</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.35">
@@ -26342,39 +26356,39 @@
       </c>
       <c r="D25" s="15">
         <f>IF(D22&lt;&gt;"",C54,"")</f>
-        <v>7.017257133649303</v>
+        <v>9.0172571336493021</v>
       </c>
       <c r="E25" s="15">
         <f t="shared" ref="E25:L27" si="4">IF(E22&lt;&gt;"",D54,"")</f>
-        <v>3.1942915791521944</v>
+        <v>7.1088601682676069</v>
       </c>
       <c r="F25" s="15">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>6.1</v>
       </c>
       <c r="G25" s="15">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>6.1</v>
       </c>
       <c r="H25" s="15">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>6.1</v>
       </c>
       <c r="I25" s="15">
         <f t="shared" si="4"/>
-        <v>-1.25</v>
+        <v>6.5047270927738641</v>
       </c>
       <c r="J25" s="15">
         <f t="shared" si="4"/>
-        <v>-2.3915375859294228</v>
+        <v>6.8881038289447343</v>
       </c>
       <c r="K25" s="15">
         <f t="shared" si="4"/>
-        <v>-3.3914802182929029</v>
+        <v>7.2503712989619817</v>
       </c>
       <c r="L25" s="15">
         <f t="shared" si="4"/>
-        <v>-4.1722365945530484</v>
+        <v>7.5937558729898971</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.35">
@@ -26391,35 +26405,35 @@
       </c>
       <c r="E26" s="15">
         <f t="shared" si="4"/>
-        <v>9.261619610847811</v>
+        <v>9.2840535147324221</v>
       </c>
       <c r="F26" s="15">
         <f t="shared" si="4"/>
-        <v>8.8688760708802157</v>
+        <v>8.9539533157165501</v>
       </c>
       <c r="G26" s="15">
         <f t="shared" si="4"/>
-        <v>8.4017965217796444</v>
+        <v>8.6237672381391697</v>
       </c>
       <c r="H26" s="15">
         <f t="shared" si="4"/>
-        <v>7.9494535507790722</v>
+        <v>8.3072267719387369</v>
       </c>
       <c r="I26" s="15">
         <f t="shared" si="4"/>
-        <v>7.5127052151790732</v>
+        <v>8.0040201590643001</v>
       </c>
       <c r="J26" s="15">
         <f t="shared" si="4"/>
-        <v>7.0278283001079238</v>
+        <v>7.7198928553946047</v>
       </c>
       <c r="K26" s="15">
         <f t="shared" si="4"/>
-        <v>6.4600038694714055</v>
+        <v>7.452338780376186</v>
       </c>
       <c r="L26" s="15">
         <f t="shared" si="4"/>
-        <v>5.733200742230979</v>
+        <v>7.2013966112482724</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.35">
@@ -26486,39 +26500,39 @@
       </c>
       <c r="D29" s="15">
         <f t="shared" ref="D29:L30" si="5">IF(D22&lt;&gt;"",$B29*D$24,"")</f>
-        <v>8.3555511600000152</v>
+        <v>9.3555511600000152</v>
       </c>
       <c r="E29" s="15">
         <f t="shared" si="5"/>
-        <v>6.2279555950000027</v>
+        <v>8.1964568415000141</v>
       </c>
       <c r="F29" s="15">
         <f t="shared" si="5"/>
-        <v>4.4344380354401078</v>
+        <v>7.5269766578582749</v>
       </c>
       <c r="G29" s="15">
         <f t="shared" si="5"/>
-        <v>4.2008982608898222</v>
+        <v>7.3618836190695847</v>
       </c>
       <c r="H29" s="15">
         <f t="shared" si="5"/>
-        <v>3.9747267753895361</v>
+        <v>7.2036133859693683</v>
       </c>
       <c r="I29" s="15">
         <f t="shared" si="5"/>
-        <v>3.1313526075895366</v>
+        <v>7.2543736259190821</v>
       </c>
       <c r="J29" s="15">
         <f t="shared" si="5"/>
-        <v>2.3181453570892505</v>
+        <v>7.3039983421696695</v>
       </c>
       <c r="K29" s="15">
         <f t="shared" si="5"/>
-        <v>1.5342618255892513</v>
+        <v>7.3513550396690839</v>
       </c>
       <c r="L29" s="15">
         <f t="shared" si="5"/>
-        <v>0.78048207383896528</v>
+        <v>7.3975762421190847</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.35">
@@ -26535,39 +26549,39 @@
       </c>
       <c r="D30" s="15">
         <f t="shared" si="5"/>
-        <v>8.3555511600000152</v>
+        <v>9.3555511600000152</v>
       </c>
       <c r="E30" s="15">
         <f t="shared" si="5"/>
-        <v>6.2279555950000027</v>
+        <v>8.1964568415000141</v>
       </c>
       <c r="F30" s="15">
         <f t="shared" si="5"/>
-        <v>4.4344380354401078</v>
+        <v>7.5269766578582749</v>
       </c>
       <c r="G30" s="15">
         <f t="shared" si="5"/>
-        <v>4.2008982608898222</v>
+        <v>7.3618836190695847</v>
       </c>
       <c r="H30" s="15">
         <f t="shared" si="5"/>
-        <v>3.9747267753895361</v>
+        <v>7.2036133859693683</v>
       </c>
       <c r="I30" s="15">
         <f t="shared" si="5"/>
-        <v>3.1313526075895366</v>
+        <v>7.2543736259190821</v>
       </c>
       <c r="J30" s="15">
         <f t="shared" si="5"/>
-        <v>2.3181453570892505</v>
+        <v>7.3039983421696695</v>
       </c>
       <c r="K30" s="15">
         <f t="shared" si="5"/>
-        <v>1.5342618255892513</v>
+        <v>7.3513550396690839</v>
       </c>
       <c r="L30" s="15">
         <f t="shared" si="5"/>
-        <v>0.78048207383896528</v>
+        <v>7.3975762421190847</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.35">
@@ -26581,39 +26595,39 @@
       </c>
       <c r="D31" s="15">
         <f>IF(D$22&lt;&gt;"",VLOOKUP(D29*1000000,'Powell-Elevation-Area'!$B$5:$D$689,3)*$B$18/1000000 + VLOOKUP(D30*1000000,'Mead-Elevation-Area'!$B$5:$D$676,3)*$C$18/1000000,"")</f>
-        <v>0.88819113000002703</v>
+        <v>0.951188637</v>
       </c>
       <c r="E31" s="15">
         <f>IF(E$22&lt;&gt;"",VLOOKUP(E29*1000000,'Powell-Elevation-Area'!$B$5:$D$689,3)*$B$18/1000000 + VLOOKUP(E30*1000000,'Mead-Elevation-Area'!$B$5:$D$676,3)*$C$18/1000000,"")</f>
-        <v>0.75279660750117305</v>
+        <v>0.87773305499997312</v>
       </c>
       <c r="F31" s="15">
         <f>IF(F$22&lt;&gt;"",VLOOKUP(F29*1000000,'Powell-Elevation-Area'!$B$5:$D$689,3)*$B$18/1000000 + VLOOKUP(F30*1000000,'Mead-Elevation-Area'!$B$5:$D$676,3)*$C$18/1000000,"")</f>
-        <v>0.63407954910057307</v>
+        <v>0.83590071750057304</v>
       </c>
       <c r="G31" s="15">
         <f>IF(G$22&lt;&gt;"",VLOOKUP(G29*1000000,'Powell-Elevation-Area'!$B$5:$D$689,3)*$B$18/1000000 + VLOOKUP(G30*1000000,'Mead-Elevation-Area'!$B$5:$D$676,3)*$C$18/1000000,"")</f>
-        <v>0.61934297100057312</v>
+        <v>0.82557159509940004</v>
       </c>
       <c r="H31" s="15">
         <f>IF(H$22&lt;&gt;"",VLOOKUP(H29*1000000,'Powell-Elevation-Area'!$B$5:$D$689,3)*$B$18/1000000 + VLOOKUP(H30*1000000,'Mead-Elevation-Area'!$B$5:$D$676,3)*$C$18/1000000,"")</f>
-        <v>0.60374833560000007</v>
+        <v>0.81547952010057301</v>
       </c>
       <c r="I31" s="15">
         <f>IF(I$22&lt;&gt;"",VLOOKUP(I29*1000000,'Powell-Elevation-Area'!$B$5:$D$689,3)*$B$18/1000000 + VLOOKUP(I30*1000000,'Mead-Elevation-Area'!$B$5:$D$676,3)*$C$18/1000000,"")</f>
-        <v>0.54341450100057298</v>
+        <v>0.81775056749882702</v>
       </c>
       <c r="J31" s="15">
         <f>IF(J$22&lt;&gt;"",VLOOKUP(J29*1000000,'Powell-Elevation-Area'!$B$5:$D$689,3)*$B$18/1000000 + VLOOKUP(J30*1000000,'Mead-Elevation-Area'!$B$5:$D$676,3)*$C$18/1000000,"")</f>
-        <v>0.484767063</v>
+        <v>0.82228660500117301</v>
       </c>
       <c r="K31" s="15">
         <f>IF(K$22&lt;&gt;"",VLOOKUP(K29*1000000,'Powell-Elevation-Area'!$B$5:$D$689,3)*$B$18/1000000 + VLOOKUP(K30*1000000,'Mead-Elevation-Area'!$B$5:$D$676,3)*$C$18/1000000,"")</f>
-        <v>0.42455950350057303</v>
+        <v>0.82455759509999993</v>
       </c>
       <c r="L31" s="15">
         <f>IF(L$22&lt;&gt;"",VLOOKUP(L29*1000000,'Powell-Elevation-Area'!$B$5:$D$689,3)*$B$18/1000000 + VLOOKUP(L30*1000000,'Mead-Elevation-Area'!$B$5:$D$676,3)*$C$18/1000000,"")</f>
-        <v>0.36617264849940001</v>
+        <v>0.82783664249940003</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.35">
@@ -26627,39 +26641,39 @@
       </c>
       <c r="D32" s="15">
         <f t="shared" ref="D32:L34" si="6">IF(D$22&lt;&gt;"",D$31*D25/D$24,"")</f>
-        <v>0.37296555449710833</v>
+        <v>0.458396965381695</v>
       </c>
       <c r="E32" s="15">
         <f t="shared" si="6"/>
-        <v>0.19305306753357929</v>
+        <v>0.38063285598410107</v>
       </c>
       <c r="F32" s="15">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>0.33871463992319345</v>
       </c>
       <c r="G32" s="15">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>0.34203112889896525</v>
       </c>
       <c r="H32" s="15">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>0.34527290722613518</v>
       </c>
       <c r="I32" s="15">
         <f t="shared" si="6"/>
-        <v>-0.10846241407057725</v>
+        <v>0.36662326382912958</v>
       </c>
       <c r="J32" s="15">
         <f t="shared" si="6"/>
-        <v>-0.25005736763651981</v>
+        <v>0.38773252998275209</v>
       </c>
       <c r="K32" s="15">
         <f t="shared" si="6"/>
-        <v>-0.46924362373985451</v>
+        <v>0.40661542597208489</v>
       </c>
       <c r="L32" s="15">
         <f t="shared" si="6"/>
-        <v>-0.97872774737733781</v>
+        <v>0.42489520622063093</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.35">
@@ -26673,39 +26687,39 @@
       </c>
       <c r="D33" s="15">
         <f t="shared" si="6"/>
-        <v>0.51522557550291859</v>
+        <v>0.49279167161830495</v>
       </c>
       <c r="E33" s="15">
         <f t="shared" si="6"/>
-        <v>0.55974353996759385</v>
+        <v>0.4971001990158721</v>
       </c>
       <c r="F33" s="15">
         <f t="shared" si="6"/>
-        <v>0.63407954910057307</v>
+        <v>0.49718607757737959</v>
       </c>
       <c r="G33" s="15">
         <f t="shared" si="6"/>
-        <v>0.61934297100057312</v>
+        <v>0.48354046620043478</v>
       </c>
       <c r="H33" s="15">
         <f t="shared" si="6"/>
-        <v>0.60374833560000007</v>
+        <v>0.47020661287443777</v>
       </c>
       <c r="I33" s="15">
         <f t="shared" si="6"/>
-        <v>0.6518769150711502</v>
+        <v>0.45112730366969739</v>
       </c>
       <c r="J33" s="15">
         <f t="shared" si="6"/>
-        <v>0.73482443063651981</v>
+        <v>0.43455407501842092</v>
       </c>
       <c r="K33" s="15">
         <f t="shared" si="6"/>
-        <v>0.89380312724042754</v>
+        <v>0.41794216912791515</v>
       </c>
       <c r="L33" s="15">
         <f t="shared" si="6"/>
-        <v>1.3449003958767378</v>
+        <v>0.40294143627876911</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.35">
@@ -26807,43 +26821,43 @@
       <c r="B36" s="1"/>
       <c r="C36" s="15">
         <f>IF(C$22&lt;&gt;"",C22-C35/2,"")</f>
-        <v>8.25</v>
+        <v>10.25</v>
       </c>
       <c r="D36" s="15">
         <f t="shared" ref="D36:L36" si="8">IF(D$22&lt;&gt;"",D22-D35/2,"")</f>
-        <v>8.25</v>
+        <v>10.25</v>
       </c>
       <c r="E36" s="15">
         <f t="shared" si="8"/>
-        <v>8.25</v>
+        <v>10.25</v>
       </c>
       <c r="F36" s="15">
         <f t="shared" si="8"/>
-        <v>8.25</v>
+        <v>10.25</v>
       </c>
       <c r="G36" s="15">
         <f t="shared" si="8"/>
-        <v>8.25</v>
+        <v>10.25</v>
       </c>
       <c r="H36" s="15">
         <f t="shared" si="8"/>
-        <v>8.25</v>
+        <v>10.25</v>
       </c>
       <c r="I36" s="15">
         <f t="shared" si="8"/>
-        <v>8.25</v>
+        <v>10.25</v>
       </c>
       <c r="J36" s="15">
         <f t="shared" si="8"/>
-        <v>8.25</v>
+        <v>10.25</v>
       </c>
       <c r="K36" s="15">
         <f t="shared" si="8"/>
-        <v>8.25</v>
+        <v>10.25</v>
       </c>
       <c r="L36" s="15">
         <f t="shared" si="8"/>
-        <v>8.25</v>
+        <v>10.25</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.35">
@@ -26853,43 +26867,43 @@
       <c r="B37" s="25"/>
       <c r="C37" s="15">
         <f>IF(C22&lt;&gt;"",MAX(0,C36-C38),"")</f>
-        <v>0.75</v>
+        <v>2.75</v>
       </c>
       <c r="D37" s="15">
         <f t="shared" ref="D37:L37" si="9">IF(D22&lt;&gt;"",MAX(0,D36-D38),"")</f>
-        <v>0.75</v>
+        <v>2.75</v>
       </c>
       <c r="E37" s="15">
         <f t="shared" si="9"/>
-        <v>0.75</v>
+        <v>2.75</v>
       </c>
       <c r="F37" s="15">
         <f t="shared" si="9"/>
-        <v>0.75</v>
+        <v>2.75</v>
       </c>
       <c r="G37" s="15">
         <f t="shared" si="9"/>
-        <v>0.75</v>
+        <v>2.75</v>
       </c>
       <c r="H37" s="15">
         <f t="shared" si="9"/>
-        <v>0.75</v>
+        <v>2.75</v>
       </c>
       <c r="I37" s="15">
         <f t="shared" si="9"/>
-        <v>0.75</v>
+        <v>2.75</v>
       </c>
       <c r="J37" s="15">
         <f t="shared" si="9"/>
-        <v>0.75</v>
+        <v>2.75</v>
       </c>
       <c r="K37" s="15">
         <f t="shared" si="9"/>
-        <v>0.75</v>
+        <v>2.75</v>
       </c>
       <c r="L37" s="15">
         <f t="shared" si="9"/>
-        <v>0.75</v>
+        <v>2.75</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.35">
@@ -27032,43 +27046,43 @@
       </c>
       <c r="C45" s="15">
         <f>IF(C$22&lt;&gt;"",C25+C37-C32-C40,"")</f>
-        <v>11.217257133649303</v>
+        <v>13.217257133649303</v>
       </c>
       <c r="D45" s="15">
         <f t="shared" ref="D45:L45" si="11">IF(D$22&lt;&gt;"",D25+D37-D32-D40,"")</f>
-        <v>7.3942915791521946</v>
+        <v>11.308860168267607</v>
       </c>
       <c r="E45" s="15">
         <f t="shared" si="11"/>
-        <v>3.7512385116186153</v>
+        <v>9.4782273122835061</v>
       </c>
       <c r="F45" s="15">
         <f>IF(F$22&lt;&gt;"",F25+F37-F32-F40,"")</f>
-        <v>0.75</v>
+        <v>8.5112853600768066</v>
       </c>
       <c r="G45" s="15">
         <f t="shared" si="11"/>
-        <v>0.75</v>
+        <v>8.5079688711010348</v>
       </c>
       <c r="H45" s="15">
         <f t="shared" si="11"/>
-        <v>0.75</v>
+        <v>8.5047270927738641</v>
       </c>
       <c r="I45" s="15">
         <f t="shared" si="11"/>
-        <v>-0.39153758592942278</v>
+        <v>8.8881038289447343</v>
       </c>
       <c r="J45" s="15">
         <f t="shared" si="11"/>
-        <v>-1.3914802182929029</v>
+        <v>9.2503712989619817</v>
       </c>
       <c r="K45" s="15">
         <f t="shared" si="11"/>
-        <v>-2.1722365945530484</v>
+        <v>9.5937558729898971</v>
       </c>
       <c r="L45" s="15">
         <f t="shared" si="11"/>
-        <v>-2.4435088471757105</v>
+        <v>9.918860666769266</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.35">
@@ -27081,39 +27095,39 @@
       </c>
       <c r="D46" s="15">
         <f t="shared" ref="D46:L46" si="12">IF(D$22&lt;&gt;"",D26+D38-D33+D40+D42+D23-D35/2,"")</f>
-        <v>16.728619610847812</v>
+        <v>16.751053514732423</v>
       </c>
       <c r="E46" s="15">
         <f t="shared" si="12"/>
-        <v>16.251876070880215</v>
+        <v>16.336953315716549</v>
       </c>
       <c r="F46" s="15">
         <f t="shared" si="12"/>
-        <v>15.784796521779644</v>
+        <v>16.006767238139169</v>
       </c>
       <c r="G46" s="15">
         <f t="shared" si="12"/>
-        <v>15.332453550779071</v>
+        <v>15.690226771938736</v>
       </c>
       <c r="H46" s="15">
         <f t="shared" si="12"/>
-        <v>14.895705215179072</v>
+        <v>15.387020159064299</v>
       </c>
       <c r="I46" s="15">
         <f t="shared" si="12"/>
-        <v>14.410828300107923</v>
+        <v>15.102892855394604</v>
       </c>
       <c r="J46" s="15">
         <f t="shared" si="12"/>
-        <v>13.843003869471405</v>
+        <v>14.835338780376185</v>
       </c>
       <c r="K46" s="15">
         <f t="shared" si="12"/>
-        <v>13.116200742230978</v>
+        <v>14.584396611248271</v>
       </c>
       <c r="L46" s="15">
         <f t="shared" si="12"/>
-        <v>11.938300346354241</v>
+        <v>14.348455174969503</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.35">
@@ -27182,24 +27196,24 @@
         <v>152</v>
       </c>
       <c r="C49" s="45">
-        <f>IF(C45&gt;4.2,4.2,C45)</f>
+        <f>IF(C45&gt;6.1+4.2,4.2,MAX(C45-6.1,0))</f>
         <v>4.2</v>
       </c>
       <c r="D49" s="45">
-        <f t="shared" ref="D49:G49" si="14">IF(D45&gt;4.2,4.2,D45)</f>
+        <f t="shared" ref="D49:G49" si="14">IF(D45&gt;6.1+4.2,4.2,MAX(D45-6.1,0))</f>
         <v>4.2</v>
       </c>
       <c r="E49" s="45">
         <f t="shared" si="14"/>
-        <v>3.7512385116186153</v>
+        <v>3.3782273122835065</v>
       </c>
       <c r="F49" s="45">
         <f t="shared" si="14"/>
-        <v>0.75</v>
+        <v>2.4112853600768069</v>
       </c>
       <c r="G49" s="45">
         <f t="shared" si="14"/>
-        <v>0.75</v>
+        <v>2.4079688711010352</v>
       </c>
       <c r="H49" s="45">
         <v>2</v>
@@ -27430,43 +27444,43 @@
       </c>
       <c r="C54" s="15">
         <f>IF(C$22&lt;&gt;"",C45-C49,"")</f>
-        <v>7.017257133649303</v>
+        <v>9.0172571336493021</v>
       </c>
       <c r="D54" s="15">
         <f t="shared" ref="D54:L54" si="19">IF(D$22&lt;&gt;"",D45-D49,"")</f>
-        <v>3.1942915791521944</v>
+        <v>7.1088601682676069</v>
       </c>
       <c r="E54" s="15">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>6.1</v>
       </c>
       <c r="F54" s="15">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>6.1</v>
       </c>
       <c r="G54" s="15">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>6.1</v>
       </c>
       <c r="H54" s="15">
         <f t="shared" si="19"/>
-        <v>-1.25</v>
+        <v>6.5047270927738641</v>
       </c>
       <c r="I54" s="15">
         <f t="shared" si="19"/>
-        <v>-2.3915375859294228</v>
+        <v>6.8881038289447343</v>
       </c>
       <c r="J54" s="15">
         <f t="shared" si="19"/>
-        <v>-3.3914802182929029</v>
+        <v>7.2503712989619817</v>
       </c>
       <c r="K54" s="15">
         <f t="shared" si="19"/>
-        <v>-4.1722365945530484</v>
+        <v>7.5937558729898971</v>
       </c>
       <c r="L54" s="15">
         <f t="shared" si="19"/>
-        <v>-4.4435088471757105</v>
+        <v>7.918860666769266</v>
       </c>
       <c r="N54" s="41">
         <v>1040</v>
@@ -27495,39 +27509,39 @@
       </c>
       <c r="D55" s="15">
         <f t="shared" ref="D55:L55" si="20">IF(D$22&lt;&gt;"",D46-D50-D51,"")</f>
-        <v>9.261619610847811</v>
+        <v>9.2840535147324221</v>
       </c>
       <c r="E55" s="15">
         <f t="shared" si="20"/>
-        <v>8.8688760708802157</v>
+        <v>8.9539533157165501</v>
       </c>
       <c r="F55" s="15">
         <f t="shared" si="20"/>
-        <v>8.4017965217796444</v>
+        <v>8.6237672381391697</v>
       </c>
       <c r="G55" s="15">
         <f t="shared" si="20"/>
-        <v>7.9494535507790722</v>
+        <v>8.3072267719387369</v>
       </c>
       <c r="H55" s="15">
         <f t="shared" si="20"/>
-        <v>7.5127052151790732</v>
+        <v>8.0040201590643001</v>
       </c>
       <c r="I55" s="15">
         <f t="shared" si="20"/>
-        <v>7.0278283001079238</v>
+        <v>7.7198928553946047</v>
       </c>
       <c r="J55" s="15">
         <f t="shared" si="20"/>
-        <v>6.4600038694714055</v>
+        <v>7.452338780376186</v>
       </c>
       <c r="K55" s="15">
         <f t="shared" si="20"/>
-        <v>5.733200742230979</v>
+        <v>7.2013966112482724</v>
       </c>
       <c r="L55" s="15">
         <f t="shared" si="20"/>
-        <v>4.5553003463542421</v>
+        <v>6.9654551749695042</v>
       </c>
       <c r="N55" s="41">
         <v>1045</v>
@@ -27614,43 +27628,43 @@
       <c r="B57" s="1"/>
       <c r="C57" s="15">
         <f>IF(C$22&lt;&gt;"",SUM(C54:C56),"")</f>
-        <v>16.71110232000003</v>
+        <v>18.71110232000003</v>
       </c>
       <c r="D57" s="15">
         <f t="shared" ref="D57:L57" si="22">IF(D$22&lt;&gt;"",SUM(D54:D56),"")</f>
-        <v>12.455911190000005</v>
+        <v>16.392913683000028</v>
       </c>
       <c r="E57" s="15">
         <f t="shared" si="22"/>
-        <v>8.8688760708802157</v>
+        <v>15.05395331571655</v>
       </c>
       <c r="F57" s="15">
         <f t="shared" si="22"/>
-        <v>8.4017965217796444</v>
+        <v>14.723767238139169</v>
       </c>
       <c r="G57" s="15">
         <f t="shared" si="22"/>
-        <v>7.9494535507790722</v>
+        <v>14.407226771938737</v>
       </c>
       <c r="H57" s="15">
         <f t="shared" si="22"/>
-        <v>6.2627052151790732</v>
+        <v>14.508747251838164</v>
       </c>
       <c r="I57" s="15">
         <f t="shared" si="22"/>
-        <v>4.636290714178501</v>
+        <v>14.607996684339339</v>
       </c>
       <c r="J57" s="15">
         <f t="shared" si="22"/>
-        <v>3.0685236511785026</v>
+        <v>14.702710079338168</v>
       </c>
       <c r="K57" s="15">
         <f t="shared" si="22"/>
-        <v>1.5609641476779306</v>
+        <v>14.795152484238169</v>
       </c>
       <c r="L57" s="15">
         <f t="shared" si="22"/>
-        <v>0.11179149917853159</v>
+        <v>14.88431584173877</v>
       </c>
       <c r="N57" s="41">
         <v>1075</v>
@@ -27908,8 +27922,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2525616F-FCF2-4465-9405-C17989B2BC95}">
   <dimension ref="A1:R62"/>
   <sheetViews>
-    <sheetView topLeftCell="B47" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49:C50"/>
+    <sheetView topLeftCell="A40" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Minor tweaks on UB depletions. Correct spelling of Millennium in worksheet names.
</commit_message>
<xml_diff>
--- a/InteractiveWaterBudget/InteractiveWaterBudget-CombinedPowellMead.xlsx
+++ b/InteractiveWaterBudget/InteractiveWaterBudget-CombinedPowellMead.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverFutures\InteractiveWaterBudget\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C254D04-C367-4FE1-B259-69C8DCC964D6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A68354B-1425-42BB-ADB3-E3B5612FF22D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6640" xr2:uid="{5373AB19-D84C-490D-97DC-C516D358024A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6640" firstSheet="5" xr2:uid="{5373AB19-D84C-490D-97DC-C516D358024A}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe-Directions" sheetId="6" r:id="rId1"/>
@@ -18,8 +18,8 @@
     <sheet name="11.0-Trade" sheetId="12" r:id="rId3"/>
     <sheet name="11.0-LawOfRiver" sheetId="13" r:id="rId4"/>
     <sheet name="11.0-Plots" sheetId="19" r:id="rId5"/>
-    <sheet name="MilleniumRecovers-LawOfRiver" sheetId="11" r:id="rId6"/>
-    <sheet name="Mill-Plots" sheetId="20" r:id="rId7"/>
+    <sheet name="MillenniumRecovers-LawOfRiver" sheetId="11" r:id="rId6"/>
+    <sheet name="Millennium-Plots" sheetId="20" r:id="rId7"/>
     <sheet name="HydrologicScenarios" sheetId="7" r:id="rId8"/>
     <sheet name="Powell-Elevation-Area" sheetId="2" r:id="rId9"/>
     <sheet name="Mead-Elevation-Area" sheetId="10" r:id="rId10"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="174">
   <si>
     <t xml:space="preserve">    To Upper Basin</t>
   </si>
@@ -484,25 +484,13 @@
     <t>11.0-LawOfRiver</t>
   </si>
   <si>
-    <t>A completed role play with Lee Ferry natural flow of 11.0 maf per year for 5 years following the Law of the River for all political decisions</t>
-  </si>
-  <si>
-    <t>A completed role play with Lee Ferry natural flow of 11.0 maf per year for 5 years allowing trades between users. Trades in Years 1 through 3 earn the Upper Basin $0.5 Billion and get the Upper Basin on a path of conservation and softer landing for this severe event.</t>
-  </si>
-  <si>
     <t xml:space="preserve">   Starting storage (million acre feet)</t>
   </si>
   <si>
     <t>MellenniumRecovery-LawOfRiver</t>
   </si>
   <si>
-    <t>A completed role play of the Millennium Drought (12.4 maf every year natural flow at Lee Ferry) for 6 years followed by 14.4 maf every year in Years 7, 8, 9, and 10. The Law of the River is followed for all political decisions.</t>
-  </si>
-  <si>
     <t>11.0-Plots</t>
-  </si>
-  <si>
-    <t>Plots of Lower and Upper Basin Consumptive Use and Account Balances that compare results for 11.0-Trade and 11.0-LawOfRiver</t>
   </si>
   <si>
     <t>Powell Release - to store physically</t>
@@ -551,6 +539,24 @@
   </si>
   <si>
     <t>This interactive water budget allows a facilitator and representatives of the Upper Basin, Lower Basin, and Mexico to role play Lake Powell and Lake Mead management year by year. A facilitator decides the hydrology to use (see HydrologicScenarios worksheet) and reveals natural inflow to Lake Powell and intervening flows along the Grand Canyon reach between Lake Powell and Lake Mead year-by-year to the players. Each player has a water storage account in the combined Lake Powell-Lake Mead system. Each year, each player’s account is credited with a portion of that year’s natural flow. The credit depends on the political decision about how to partition natural flow among the players and subtracts the player's share of reservoir evaporation. The player’s share of reservoir evaporation is prorated by their and aggregate account balances. Each year, each player decides the volume to consumptively use (deduct from their account) and water to store/conserve (remains in the account). A player’s consumptive use must stay within their available water. Additionally, the Upper Basin player can voluntarily trade and transfer stored water to the Lower Basin player with compensation. The Mexico player can also voluntarily trade and transfer stored water to the Lower Basin player with compensation. The trades move water from one account to another; trades do not change physical storage. Finally, the interactive water budget calculates each player’s end-of-the-year account balance. The tool also applies a political decision of how to physically split and move the total storage – sum of all account balances – between Lake Powell and Lake Mead. The players then move to the next year and repeat the decision steps.</t>
+  </si>
+  <si>
+    <t>A completed role play with Lee Ferry natural flow of 11.0 maf every year for 5 years allowing trades between users. Trades in Years 1 through 3 earn the Upper Basin $0.46 Billion and get the Upper Basin on a path of conservation and softer landing for this severe event.</t>
+  </si>
+  <si>
+    <t>A completed role play with Lee Ferry natural flow of 11.0 maf every year for 5 years and all political decisions follow the existing Law of the River operations (DCP, Equalization, Curtailment)</t>
+  </si>
+  <si>
+    <t>Plots of Lower and Upper Basin Consumptive Use and Account Balances that compare results for 11.0-Trade and 11.0-LawOfRiver operations</t>
+  </si>
+  <si>
+    <t>A completed role play of the Millennium Drought (12.4 maf every year natural flow at Lee Ferry) for 6 years followed by 14.4 maf every year in Years 7, 8, 9, and 10. All political decisions follow the the existing Law of the River operations (DCPs, Equalization, Curtailment).</t>
+  </si>
+  <si>
+    <t>Mead-Elevation-Area</t>
+  </si>
+  <si>
+    <t>The Lake Mead storage volume-elevation-area curve data downloaded from CRSS.</t>
   </si>
 </sst>
 </file>
@@ -923,6 +929,8 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -959,8 +967,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2122,13 +2128,13 @@
                   <c:v>3.3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.9</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.7</c:v>
+                  <c:v>2.8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.7</c:v>
+                  <c:v>2.8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6811,10 +6817,10 @@
                   <c:v>7.6634520548331819</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.7418099968023153</c:v>
+                  <c:v>6.6418099968023157</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.4602708271803406</c:v>
+                  <c:v>6.2648771960174221</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7751,7 +7757,7 @@
                   <c:v>10.193338646698306</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9.7622661278208565</c:v>
+                  <c:v>9.7612192784826295</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8019,7 +8025,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'MilleniumRecovers-LawOfRiver'!$C$21:$L$21</c:f>
+              <c:f>'MillenniumRecovers-LawOfRiver'!$C$21:$L$21</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
@@ -8057,7 +8063,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'MilleniumRecovers-LawOfRiver'!$C$50:$L$50</c:f>
+              <c:f>'MillenniumRecovers-LawOfRiver'!$C$50:$L$50</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="10"/>
@@ -8134,7 +8140,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'MilleniumRecovers-LawOfRiver'!$C$21:$L$21</c:f>
+              <c:f>'MillenniumRecovers-LawOfRiver'!$C$21:$L$21</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
@@ -8172,7 +8178,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'MilleniumRecovers-LawOfRiver'!$C$49:$L$49</c:f>
+              <c:f>'MillenniumRecovers-LawOfRiver'!$C$49:$L$49</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="10"/>
@@ -8588,7 +8594,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'MilleniumRecovers-LawOfRiver'!$C$21:$L$21</c:f>
+              <c:f>'MillenniumRecovers-LawOfRiver'!$C$21:$L$21</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
@@ -8626,7 +8632,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'MilleniumRecovers-LawOfRiver'!$C$26:$L$26</c:f>
+              <c:f>'MillenniumRecovers-LawOfRiver'!$C$26:$L$26</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="10"/>
@@ -8703,7 +8709,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'MilleniumRecovers-LawOfRiver'!$C$21:$L$21</c:f>
+              <c:f>'MillenniumRecovers-LawOfRiver'!$C$21:$L$21</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
@@ -8741,7 +8747,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'MilleniumRecovers-LawOfRiver'!$C$25:$L$25</c:f>
+              <c:f>'MillenniumRecovers-LawOfRiver'!$C$25:$L$25</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="10"/>
@@ -25977,8 +25983,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{447CC9A2-4C52-453A-A3CD-EA6E59E26162}">
   <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -26018,20 +26024,20 @@
       <c r="D3"/>
     </row>
     <row r="4" spans="1:12" ht="187.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="63" t="s">
-        <v>171</v>
-      </c>
-      <c r="B4" s="63"/>
-      <c r="C4" s="63"/>
-      <c r="D4" s="63"/>
-      <c r="E4" s="63"/>
-      <c r="F4" s="63"/>
-      <c r="G4" s="63"/>
-      <c r="H4" s="63"/>
-      <c r="I4" s="63"/>
-      <c r="J4" s="63"/>
-      <c r="K4" s="63"/>
-      <c r="L4" s="63"/>
+      <c r="A4" s="65" t="s">
+        <v>167</v>
+      </c>
+      <c r="B4" s="65"/>
+      <c r="C4" s="65"/>
+      <c r="D4" s="65"/>
+      <c r="E4" s="65"/>
+      <c r="F4" s="65"/>
+      <c r="G4" s="65"/>
+      <c r="H4" s="65"/>
+      <c r="I4" s="65"/>
+      <c r="J4" s="65"/>
+      <c r="K4" s="65"/>
+      <c r="L4" s="65"/>
     </row>
     <row r="5" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="16"/>
@@ -26047,254 +26053,254 @@
       <c r="L5" s="16"/>
     </row>
     <row r="6" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="54" t="s">
+      <c r="A6" s="56" t="s">
         <v>113</v>
       </c>
-      <c r="B6" s="55"/>
-      <c r="C6" s="55"/>
-      <c r="D6" s="55"/>
-      <c r="E6" s="55"/>
-      <c r="F6" s="55"/>
-      <c r="G6" s="55"/>
-      <c r="H6" s="55"/>
-      <c r="I6" s="55"/>
-      <c r="J6" s="55"/>
-      <c r="K6" s="55"/>
-      <c r="L6" s="56"/>
+      <c r="B6" s="57"/>
+      <c r="C6" s="57"/>
+      <c r="D6" s="57"/>
+      <c r="E6" s="57"/>
+      <c r="F6" s="57"/>
+      <c r="G6" s="57"/>
+      <c r="H6" s="57"/>
+      <c r="I6" s="57"/>
+      <c r="J6" s="57"/>
+      <c r="K6" s="57"/>
+      <c r="L6" s="58"/>
     </row>
     <row r="7" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="29">
         <v>1</v>
       </c>
-      <c r="B7" s="57" t="s">
-        <v>160</v>
-      </c>
-      <c r="C7" s="57"/>
-      <c r="D7" s="57"/>
-      <c r="E7" s="57"/>
-      <c r="F7" s="57"/>
-      <c r="G7" s="57"/>
-      <c r="H7" s="57"/>
-      <c r="I7" s="57"/>
-      <c r="J7" s="57"/>
-      <c r="K7" s="57"/>
-      <c r="L7" s="58"/>
+      <c r="B7" s="59" t="s">
+        <v>156</v>
+      </c>
+      <c r="C7" s="59"/>
+      <c r="D7" s="59"/>
+      <c r="E7" s="59"/>
+      <c r="F7" s="59"/>
+      <c r="G7" s="59"/>
+      <c r="H7" s="59"/>
+      <c r="I7" s="59"/>
+      <c r="J7" s="59"/>
+      <c r="K7" s="59"/>
+      <c r="L7" s="60"/>
     </row>
     <row r="8" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="29">
         <v>2</v>
       </c>
-      <c r="B8" s="57" t="s">
+      <c r="B8" s="59" t="s">
         <v>95</v>
       </c>
-      <c r="C8" s="57"/>
-      <c r="D8" s="57"/>
-      <c r="E8" s="57"/>
-      <c r="F8" s="57"/>
-      <c r="G8" s="57"/>
-      <c r="H8" s="57"/>
-      <c r="I8" s="57"/>
-      <c r="J8" s="57"/>
-      <c r="K8" s="57"/>
-      <c r="L8" s="58"/>
+      <c r="C8" s="59"/>
+      <c r="D8" s="59"/>
+      <c r="E8" s="59"/>
+      <c r="F8" s="59"/>
+      <c r="G8" s="59"/>
+      <c r="H8" s="59"/>
+      <c r="I8" s="59"/>
+      <c r="J8" s="59"/>
+      <c r="K8" s="59"/>
+      <c r="L8" s="60"/>
     </row>
     <row r="9" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="29">
         <v>3</v>
       </c>
-      <c r="B9" s="57" t="s">
-        <v>161</v>
-      </c>
-      <c r="C9" s="57"/>
-      <c r="D9" s="57"/>
-      <c r="E9" s="57"/>
-      <c r="F9" s="57"/>
-      <c r="G9" s="57"/>
-      <c r="H9" s="57"/>
-      <c r="I9" s="57"/>
-      <c r="J9" s="57"/>
-      <c r="K9" s="57"/>
-      <c r="L9" s="58"/>
+      <c r="B9" s="59" t="s">
+        <v>157</v>
+      </c>
+      <c r="C9" s="59"/>
+      <c r="D9" s="59"/>
+      <c r="E9" s="59"/>
+      <c r="F9" s="59"/>
+      <c r="G9" s="59"/>
+      <c r="H9" s="59"/>
+      <c r="I9" s="59"/>
+      <c r="J9" s="59"/>
+      <c r="K9" s="59"/>
+      <c r="L9" s="60"/>
     </row>
     <row r="10" spans="1:12" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="29">
         <v>4</v>
       </c>
-      <c r="B10" s="57" t="s">
+      <c r="B10" s="59" t="s">
         <v>96</v>
       </c>
-      <c r="C10" s="57"/>
-      <c r="D10" s="57"/>
-      <c r="E10" s="57"/>
-      <c r="F10" s="57"/>
-      <c r="G10" s="57"/>
-      <c r="H10" s="57"/>
-      <c r="I10" s="57"/>
-      <c r="J10" s="57"/>
-      <c r="K10" s="57"/>
-      <c r="L10" s="58"/>
+      <c r="C10" s="59"/>
+      <c r="D10" s="59"/>
+      <c r="E10" s="59"/>
+      <c r="F10" s="59"/>
+      <c r="G10" s="59"/>
+      <c r="H10" s="59"/>
+      <c r="I10" s="59"/>
+      <c r="J10" s="59"/>
+      <c r="K10" s="59"/>
+      <c r="L10" s="60"/>
     </row>
     <row r="11" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="29">
         <v>5</v>
       </c>
-      <c r="B11" s="57" t="s">
-        <v>162</v>
-      </c>
-      <c r="C11" s="57"/>
-      <c r="D11" s="57"/>
-      <c r="E11" s="57"/>
-      <c r="F11" s="57"/>
-      <c r="G11" s="57"/>
-      <c r="H11" s="57"/>
-      <c r="I11" s="57"/>
-      <c r="J11" s="57"/>
-      <c r="K11" s="57"/>
-      <c r="L11" s="58"/>
+      <c r="B11" s="59" t="s">
+        <v>158</v>
+      </c>
+      <c r="C11" s="59"/>
+      <c r="D11" s="59"/>
+      <c r="E11" s="59"/>
+      <c r="F11" s="59"/>
+      <c r="G11" s="59"/>
+      <c r="H11" s="59"/>
+      <c r="I11" s="59"/>
+      <c r="J11" s="59"/>
+      <c r="K11" s="59"/>
+      <c r="L11" s="60"/>
     </row>
     <row r="12" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="29">
         <v>6</v>
       </c>
-      <c r="B12" s="57" t="s">
-        <v>163</v>
-      </c>
-      <c r="C12" s="57"/>
-      <c r="D12" s="57"/>
-      <c r="E12" s="57"/>
-      <c r="F12" s="57"/>
-      <c r="G12" s="57"/>
-      <c r="H12" s="57"/>
-      <c r="I12" s="57"/>
-      <c r="J12" s="57"/>
-      <c r="K12" s="57"/>
-      <c r="L12" s="58"/>
+      <c r="B12" s="59" t="s">
+        <v>159</v>
+      </c>
+      <c r="C12" s="59"/>
+      <c r="D12" s="59"/>
+      <c r="E12" s="59"/>
+      <c r="F12" s="59"/>
+      <c r="G12" s="59"/>
+      <c r="H12" s="59"/>
+      <c r="I12" s="59"/>
+      <c r="J12" s="59"/>
+      <c r="K12" s="59"/>
+      <c r="L12" s="60"/>
     </row>
     <row r="13" spans="1:12" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="29">
         <v>7</v>
       </c>
-      <c r="B13" s="57" t="s">
-        <v>164</v>
-      </c>
-      <c r="C13" s="57"/>
-      <c r="D13" s="57"/>
-      <c r="E13" s="57"/>
-      <c r="F13" s="57"/>
-      <c r="G13" s="57"/>
-      <c r="H13" s="57"/>
-      <c r="I13" s="57"/>
-      <c r="J13" s="57"/>
-      <c r="K13" s="57"/>
-      <c r="L13" s="58"/>
+      <c r="B13" s="59" t="s">
+        <v>160</v>
+      </c>
+      <c r="C13" s="59"/>
+      <c r="D13" s="59"/>
+      <c r="E13" s="59"/>
+      <c r="F13" s="59"/>
+      <c r="G13" s="59"/>
+      <c r="H13" s="59"/>
+      <c r="I13" s="59"/>
+      <c r="J13" s="59"/>
+      <c r="K13" s="59"/>
+      <c r="L13" s="60"/>
     </row>
     <row r="14" spans="1:12" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="29">
         <v>8</v>
       </c>
-      <c r="B14" s="57" t="s">
-        <v>165</v>
-      </c>
-      <c r="C14" s="57"/>
-      <c r="D14" s="57"/>
-      <c r="E14" s="57"/>
-      <c r="F14" s="57"/>
-      <c r="G14" s="57"/>
-      <c r="H14" s="57"/>
-      <c r="I14" s="57"/>
-      <c r="J14" s="57"/>
-      <c r="K14" s="57"/>
-      <c r="L14" s="58"/>
+      <c r="B14" s="59" t="s">
+        <v>161</v>
+      </c>
+      <c r="C14" s="59"/>
+      <c r="D14" s="59"/>
+      <c r="E14" s="59"/>
+      <c r="F14" s="59"/>
+      <c r="G14" s="59"/>
+      <c r="H14" s="59"/>
+      <c r="I14" s="59"/>
+      <c r="J14" s="59"/>
+      <c r="K14" s="59"/>
+      <c r="L14" s="60"/>
     </row>
     <row r="15" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="29">
         <v>9</v>
       </c>
-      <c r="B15" s="57" t="s">
-        <v>166</v>
-      </c>
-      <c r="C15" s="57"/>
-      <c r="D15" s="57"/>
-      <c r="E15" s="57"/>
-      <c r="F15" s="57"/>
-      <c r="G15" s="57"/>
-      <c r="H15" s="57"/>
-      <c r="I15" s="57"/>
-      <c r="J15" s="57"/>
-      <c r="K15" s="57"/>
-      <c r="L15" s="58"/>
+      <c r="B15" s="59" t="s">
+        <v>162</v>
+      </c>
+      <c r="C15" s="59"/>
+      <c r="D15" s="59"/>
+      <c r="E15" s="59"/>
+      <c r="F15" s="59"/>
+      <c r="G15" s="59"/>
+      <c r="H15" s="59"/>
+      <c r="I15" s="59"/>
+      <c r="J15" s="59"/>
+      <c r="K15" s="59"/>
+      <c r="L15" s="60"/>
     </row>
     <row r="16" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="29">
         <v>10</v>
       </c>
-      <c r="B16" s="57" t="s">
-        <v>167</v>
-      </c>
-      <c r="C16" s="57"/>
-      <c r="D16" s="57"/>
-      <c r="E16" s="57"/>
-      <c r="F16" s="57"/>
-      <c r="G16" s="57"/>
-      <c r="H16" s="57"/>
-      <c r="I16" s="57"/>
-      <c r="J16" s="57"/>
-      <c r="K16" s="57"/>
-      <c r="L16" s="58"/>
+      <c r="B16" s="59" t="s">
+        <v>163</v>
+      </c>
+      <c r="C16" s="59"/>
+      <c r="D16" s="59"/>
+      <c r="E16" s="59"/>
+      <c r="F16" s="59"/>
+      <c r="G16" s="59"/>
+      <c r="H16" s="59"/>
+      <c r="I16" s="59"/>
+      <c r="J16" s="59"/>
+      <c r="K16" s="59"/>
+      <c r="L16" s="60"/>
     </row>
     <row r="17" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="29">
         <v>11</v>
       </c>
-      <c r="B17" s="57" t="s">
+      <c r="B17" s="59" t="s">
         <v>56</v>
       </c>
-      <c r="C17" s="57"/>
-      <c r="D17" s="57"/>
-      <c r="E17" s="57"/>
-      <c r="F17" s="57"/>
-      <c r="G17" s="57"/>
-      <c r="H17" s="57"/>
-      <c r="I17" s="57"/>
-      <c r="J17" s="57"/>
-      <c r="K17" s="57"/>
-      <c r="L17" s="58"/>
+      <c r="C17" s="59"/>
+      <c r="D17" s="59"/>
+      <c r="E17" s="59"/>
+      <c r="F17" s="59"/>
+      <c r="G17" s="59"/>
+      <c r="H17" s="59"/>
+      <c r="I17" s="59"/>
+      <c r="J17" s="59"/>
+      <c r="K17" s="59"/>
+      <c r="L17" s="60"/>
     </row>
     <row r="18" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="29">
         <v>12</v>
       </c>
-      <c r="B18" s="59" t="s">
-        <v>168</v>
-      </c>
-      <c r="C18" s="59"/>
-      <c r="D18" s="59"/>
-      <c r="E18" s="59"/>
-      <c r="F18" s="59"/>
-      <c r="G18" s="59"/>
-      <c r="H18" s="59"/>
-      <c r="I18" s="59"/>
-      <c r="J18" s="59"/>
-      <c r="K18" s="59"/>
-      <c r="L18" s="60"/>
+      <c r="B18" s="61" t="s">
+        <v>164</v>
+      </c>
+      <c r="C18" s="61"/>
+      <c r="D18" s="61"/>
+      <c r="E18" s="61"/>
+      <c r="F18" s="61"/>
+      <c r="G18" s="61"/>
+      <c r="H18" s="61"/>
+      <c r="I18" s="61"/>
+      <c r="J18" s="61"/>
+      <c r="K18" s="61"/>
+      <c r="L18" s="62"/>
     </row>
     <row r="19" spans="1:12" ht="32" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="29">
         <v>13</v>
       </c>
-      <c r="B19" s="61" t="s">
-        <v>169</v>
-      </c>
-      <c r="C19" s="61"/>
-      <c r="D19" s="61"/>
-      <c r="E19" s="61"/>
-      <c r="F19" s="61"/>
-      <c r="G19" s="61"/>
-      <c r="H19" s="61"/>
-      <c r="I19" s="61"/>
-      <c r="J19" s="61"/>
-      <c r="K19" s="61"/>
-      <c r="L19" s="62"/>
+      <c r="B19" s="63" t="s">
+        <v>165</v>
+      </c>
+      <c r="C19" s="63"/>
+      <c r="D19" s="63"/>
+      <c r="E19" s="63"/>
+      <c r="F19" s="63"/>
+      <c r="G19" s="63"/>
+      <c r="H19" s="63"/>
+      <c r="I19" s="63"/>
+      <c r="J19" s="63"/>
+      <c r="K19" s="63"/>
+      <c r="L19" s="64"/>
     </row>
     <row r="20" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B20" s="27"/>
@@ -26327,7 +26333,7 @@
         <v>147</v>
       </c>
       <c r="C23" t="s">
-        <v>150</v>
+        <v>168</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.35">
@@ -26335,23 +26341,23 @@
         <v>148</v>
       </c>
       <c r="C24" t="s">
-        <v>149</v>
+        <v>169</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B25" s="2" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C25" t="s">
-        <v>155</v>
+        <v>170</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B26" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C26" t="s">
-        <v>153</v>
+        <v>171</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.35">
@@ -26370,26 +26376,34 @@
         <v>103</v>
       </c>
     </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B29" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="C29" t="s">
+        <v>173</v>
+      </c>
+    </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="32" spans="1:12" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="53" t="s">
-        <v>170</v>
-      </c>
-      <c r="B32" s="53"/>
-      <c r="C32" s="53"/>
-      <c r="D32" s="53"/>
-      <c r="E32" s="53"/>
-      <c r="F32" s="53"/>
-      <c r="G32" s="53"/>
-      <c r="H32" s="53"/>
-      <c r="I32" s="53"/>
-      <c r="J32" s="53"/>
-      <c r="K32" s="53"/>
-      <c r="L32" s="53"/>
+      <c r="A32" s="55" t="s">
+        <v>166</v>
+      </c>
+      <c r="B32" s="55"/>
+      <c r="C32" s="55"/>
+      <c r="D32" s="55"/>
+      <c r="E32" s="55"/>
+      <c r="F32" s="55"/>
+      <c r="G32" s="55"/>
+      <c r="H32" s="55"/>
+      <c r="I32" s="55"/>
+      <c r="J32" s="55"/>
+      <c r="K32" s="55"/>
+      <c r="L32" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="16">
@@ -38728,48 +38742,48 @@
         <v>53</v>
       </c>
       <c r="B5" s="52"/>
-      <c r="C5" s="64"/>
-      <c r="D5" s="64"/>
-      <c r="E5" s="64"/>
-      <c r="F5" s="64"/>
-      <c r="G5" s="64"/>
-      <c r="H5" s="64"/>
+      <c r="C5" s="66"/>
+      <c r="D5" s="66"/>
+      <c r="E5" s="66"/>
+      <c r="F5" s="66"/>
+      <c r="G5" s="66"/>
+      <c r="H5" s="66"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="17" t="s">
         <v>41</v>
       </c>
       <c r="B6" s="52"/>
-      <c r="C6" s="64"/>
-      <c r="D6" s="64"/>
-      <c r="E6" s="64"/>
-      <c r="F6" s="64"/>
-      <c r="G6" s="64"/>
-      <c r="H6" s="64"/>
+      <c r="C6" s="66"/>
+      <c r="D6" s="66"/>
+      <c r="E6" s="66"/>
+      <c r="F6" s="66"/>
+      <c r="G6" s="66"/>
+      <c r="H6" s="66"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="17" t="s">
         <v>42</v>
       </c>
       <c r="B7" s="52"/>
-      <c r="C7" s="64"/>
-      <c r="D7" s="64"/>
-      <c r="E7" s="64"/>
-      <c r="F7" s="64"/>
-      <c r="G7" s="64"/>
-      <c r="H7" s="64"/>
+      <c r="C7" s="66"/>
+      <c r="D7" s="66"/>
+      <c r="E7" s="66"/>
+      <c r="F7" s="66"/>
+      <c r="G7" s="66"/>
+      <c r="H7" s="66"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="17" t="s">
         <v>43</v>
       </c>
       <c r="B8" s="52"/>
-      <c r="C8" s="64"/>
-      <c r="D8" s="64"/>
-      <c r="E8" s="64"/>
-      <c r="F8" s="64"/>
-      <c r="G8" s="64"/>
-      <c r="H8" s="64"/>
+      <c r="C8" s="66"/>
+      <c r="D8" s="66"/>
+      <c r="E8" s="66"/>
+      <c r="F8" s="66"/>
+      <c r="G8" s="66"/>
+      <c r="H8" s="66"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="17"/>
@@ -40662,48 +40676,48 @@
         <v>53</v>
       </c>
       <c r="B5" s="13"/>
-      <c r="C5" s="64"/>
-      <c r="D5" s="64"/>
-      <c r="E5" s="64"/>
-      <c r="F5" s="64"/>
-      <c r="G5" s="64"/>
-      <c r="H5" s="64"/>
+      <c r="C5" s="66"/>
+      <c r="D5" s="66"/>
+      <c r="E5" s="66"/>
+      <c r="F5" s="66"/>
+      <c r="G5" s="66"/>
+      <c r="H5" s="66"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="17" t="s">
         <v>41</v>
       </c>
       <c r="B6" s="13"/>
-      <c r="C6" s="64"/>
-      <c r="D6" s="64"/>
-      <c r="E6" s="64"/>
-      <c r="F6" s="64"/>
-      <c r="G6" s="64"/>
-      <c r="H6" s="64"/>
+      <c r="C6" s="66"/>
+      <c r="D6" s="66"/>
+      <c r="E6" s="66"/>
+      <c r="F6" s="66"/>
+      <c r="G6" s="66"/>
+      <c r="H6" s="66"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="17" t="s">
         <v>42</v>
       </c>
       <c r="B7" s="13"/>
-      <c r="C7" s="64"/>
-      <c r="D7" s="64"/>
-      <c r="E7" s="64"/>
-      <c r="F7" s="64"/>
-      <c r="G7" s="64"/>
-      <c r="H7" s="64"/>
+      <c r="C7" s="66"/>
+      <c r="D7" s="66"/>
+      <c r="E7" s="66"/>
+      <c r="F7" s="66"/>
+      <c r="G7" s="66"/>
+      <c r="H7" s="66"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="17" t="s">
         <v>43</v>
       </c>
       <c r="B8" s="13"/>
-      <c r="C8" s="64"/>
-      <c r="D8" s="64"/>
-      <c r="E8" s="64"/>
-      <c r="F8" s="64"/>
-      <c r="G8" s="64"/>
-      <c r="H8" s="64"/>
+      <c r="C8" s="66"/>
+      <c r="D8" s="66"/>
+      <c r="E8" s="66"/>
+      <c r="F8" s="66"/>
+      <c r="G8" s="66"/>
+      <c r="H8" s="66"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="17"/>
@@ -40766,7 +40780,7 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B19" s="12">
         <v>11</v>
@@ -42225,7 +42239,7 @@
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B58" s="1"/>
       <c r="C58" s="15" t="str">
@@ -42233,7 +42247,7 @@
         <v/>
       </c>
       <c r="D58" s="15" t="str">
-        <f t="shared" ref="D58:M58" si="24">IF(D22&lt;&gt;"",D29+D22-D32-D49-D57*$B$29,"")</f>
+        <f t="shared" ref="D58:L58" si="24">IF(D22&lt;&gt;"",D29+D22-D32-D49-D57*$B$29,"")</f>
         <v/>
       </c>
       <c r="E58" s="15" t="str">
@@ -42333,43 +42347,43 @@
         <v>132</v>
       </c>
       <c r="C61" s="15" t="str">
-        <f>IF(C$22&lt;&gt;"",C50+C60,"")</f>
+        <f t="shared" ref="C61:L61" si="26">IF(C$22&lt;&gt;"",C50+C60,"")</f>
         <v/>
       </c>
       <c r="D61" s="15" t="str">
-        <f>IF(D$22&lt;&gt;"",D50+D60,"")</f>
+        <f t="shared" si="26"/>
         <v/>
       </c>
       <c r="E61" s="15" t="str">
-        <f>IF(E$22&lt;&gt;"",E50+E60,"")</f>
+        <f t="shared" si="26"/>
         <v/>
       </c>
       <c r="F61" s="15" t="str">
-        <f>IF(F$22&lt;&gt;"",F50+F60,"")</f>
+        <f t="shared" si="26"/>
         <v/>
       </c>
       <c r="G61" s="15" t="str">
-        <f>IF(G$22&lt;&gt;"",G50+G60,"")</f>
+        <f t="shared" si="26"/>
         <v/>
       </c>
       <c r="H61" s="15">
-        <f>IF(H$22&lt;&gt;"",H50+H60,"")</f>
+        <f t="shared" si="26"/>
         <v>0.2</v>
       </c>
       <c r="I61" s="15">
-        <f>IF(I$22&lt;&gt;"",I50+I60,"")</f>
+        <f t="shared" si="26"/>
         <v>0.2</v>
       </c>
       <c r="J61" s="15">
-        <f>IF(J$22&lt;&gt;"",J50+J60,"")</f>
+        <f t="shared" si="26"/>
         <v>0.2</v>
       </c>
       <c r="K61" s="15">
-        <f>IF(K$22&lt;&gt;"",K50+K60,"")</f>
+        <f t="shared" si="26"/>
         <v>0.2</v>
       </c>
       <c r="L61" s="15">
-        <f>IF(L$22&lt;&gt;"",L50+L60,"")</f>
+        <f t="shared" si="26"/>
         <v>0.2</v>
       </c>
     </row>
@@ -42561,8 +42575,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{710BD1F0-C024-4B0C-A52B-7568661161E6}">
   <dimension ref="A1:R63"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C59" sqref="C59:G59"/>
+    <sheetView topLeftCell="A38" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -42625,48 +42639,48 @@
         <v>53</v>
       </c>
       <c r="B5" s="50"/>
-      <c r="C5" s="64"/>
-      <c r="D5" s="64"/>
-      <c r="E5" s="64"/>
-      <c r="F5" s="64"/>
-      <c r="G5" s="64"/>
-      <c r="H5" s="64"/>
+      <c r="C5" s="66"/>
+      <c r="D5" s="66"/>
+      <c r="E5" s="66"/>
+      <c r="F5" s="66"/>
+      <c r="G5" s="66"/>
+      <c r="H5" s="66"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="17" t="s">
         <v>41</v>
       </c>
       <c r="B6" s="50"/>
-      <c r="C6" s="64"/>
-      <c r="D6" s="64"/>
-      <c r="E6" s="64"/>
-      <c r="F6" s="64"/>
-      <c r="G6" s="64"/>
-      <c r="H6" s="64"/>
+      <c r="C6" s="66"/>
+      <c r="D6" s="66"/>
+      <c r="E6" s="66"/>
+      <c r="F6" s="66"/>
+      <c r="G6" s="66"/>
+      <c r="H6" s="66"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="17" t="s">
         <v>42</v>
       </c>
       <c r="B7" s="50"/>
-      <c r="C7" s="64"/>
-      <c r="D7" s="64"/>
-      <c r="E7" s="64"/>
-      <c r="F7" s="64"/>
-      <c r="G7" s="64"/>
-      <c r="H7" s="64"/>
+      <c r="C7" s="66"/>
+      <c r="D7" s="66"/>
+      <c r="E7" s="66"/>
+      <c r="F7" s="66"/>
+      <c r="G7" s="66"/>
+      <c r="H7" s="66"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="17" t="s">
         <v>43</v>
       </c>
       <c r="B8" s="50"/>
-      <c r="C8" s="64"/>
-      <c r="D8" s="64"/>
-      <c r="E8" s="64"/>
-      <c r="F8" s="64"/>
-      <c r="G8" s="64"/>
-      <c r="H8" s="64"/>
+      <c r="C8" s="66"/>
+      <c r="D8" s="66"/>
+      <c r="E8" s="66"/>
+      <c r="F8" s="66"/>
+      <c r="G8" s="66"/>
+      <c r="H8" s="66"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="17"/>
@@ -42729,7 +42743,7 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B19" s="12">
         <v>11</v>
@@ -42892,31 +42906,31 @@
       </c>
       <c r="F24" s="15">
         <f t="shared" si="3"/>
-        <v>16.935148643500622</v>
+        <v>16.835148643500624</v>
       </c>
       <c r="G24" s="15">
         <f t="shared" si="3"/>
-        <v>16.222536955001196</v>
+        <v>16.026096474500051</v>
       </c>
       <c r="H24" s="15">
         <f t="shared" si="3"/>
-        <v>15.532489937502369</v>
+        <v>15.24199254190065</v>
       </c>
       <c r="I24" s="15">
         <f t="shared" si="3"/>
-        <v>15.583530117402967</v>
+        <v>15.303535786901246</v>
       </c>
       <c r="J24" s="15">
         <f t="shared" si="3"/>
-        <v>15.633484297302365</v>
+        <v>15.362814041802418</v>
       </c>
       <c r="K24" s="15">
         <f t="shared" si="3"/>
-        <v>15.682181429801767</v>
+        <v>15.420835249303588</v>
       </c>
       <c r="L24" s="15">
         <f t="shared" si="3"/>
-        <v>15.728535572202338</v>
+        <v>15.476585466702987</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.35">
@@ -42937,31 +42951,31 @@
       </c>
       <c r="F25" s="15">
         <f t="shared" si="4"/>
-        <v>6.7418099968023153</v>
+        <v>6.6418099968023157</v>
       </c>
       <c r="G25" s="15">
         <f t="shared" si="4"/>
-        <v>6.4602708271803406</v>
+        <v>6.2648771960174221</v>
       </c>
       <c r="H25" s="15">
         <f t="shared" si="4"/>
-        <v>6.1875989313758</v>
+        <v>5.9009113310257435</v>
       </c>
       <c r="I25" s="15">
         <f t="shared" si="4"/>
-        <v>6.6332080356705205</v>
+        <v>6.3601427881994557</v>
       </c>
       <c r="J25" s="15">
         <f t="shared" si="4"/>
-        <v>7.0551047884565037</v>
+        <v>6.7944923994879503</v>
       </c>
       <c r="K25" s="15">
         <f t="shared" si="4"/>
-        <v>7.4545735699081455</v>
+        <v>7.2057846941326744</v>
       </c>
       <c r="L25" s="15">
         <f t="shared" si="4"/>
-        <v>7.8323643052138578</v>
+        <v>7.5948852881101416</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.35">
@@ -42986,27 +43000,27 @@
       </c>
       <c r="G26" s="15">
         <f t="shared" si="4"/>
-        <v>9.7622661278208565</v>
+        <v>9.7612192784826295</v>
       </c>
       <c r="H26" s="15">
         <f t="shared" si="4"/>
-        <v>9.3448910061265682</v>
+        <v>9.3410812108749059</v>
       </c>
       <c r="I26" s="15">
         <f t="shared" si="4"/>
-        <v>8.9503220817324465</v>
+        <v>8.9433929987017908</v>
       </c>
       <c r="J26" s="15">
         <f t="shared" si="4"/>
-        <v>8.5783795088458614</v>
+        <v>8.5683216423144675</v>
       </c>
       <c r="K26" s="15">
         <f t="shared" si="4"/>
-        <v>8.227607859893622</v>
+        <v>8.2150505551709134</v>
       </c>
       <c r="L26" s="15">
         <f t="shared" si="4"/>
-        <v>7.89617126698848</v>
+        <v>7.8817001785928458</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.35">
@@ -43081,31 +43095,31 @@
       </c>
       <c r="F29" s="15">
         <f t="shared" si="5"/>
-        <v>8.4675743217503108</v>
+        <v>8.4175743217503118</v>
       </c>
       <c r="G29" s="15">
         <f t="shared" si="5"/>
-        <v>8.1112684775005981</v>
+        <v>8.0130482372500254</v>
       </c>
       <c r="H29" s="15">
         <f t="shared" si="5"/>
-        <v>7.7662449687511845</v>
+        <v>7.6209962709503252</v>
       </c>
       <c r="I29" s="15">
         <f t="shared" si="5"/>
-        <v>7.7917650587014835</v>
+        <v>7.6517678934506232</v>
       </c>
       <c r="J29" s="15">
         <f t="shared" si="5"/>
-        <v>7.8167421486511826</v>
+        <v>7.6814070209012089</v>
       </c>
       <c r="K29" s="15">
         <f t="shared" si="5"/>
-        <v>7.8410907149008837</v>
+        <v>7.7104176246517939</v>
       </c>
       <c r="L29" s="15">
         <f t="shared" si="5"/>
-        <v>7.8642677861011689</v>
+        <v>7.7382927333514937</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.35">
@@ -43130,31 +43144,31 @@
       </c>
       <c r="F30" s="15">
         <f t="shared" si="5"/>
-        <v>8.4675743217503108</v>
+        <v>8.4175743217503118</v>
       </c>
       <c r="G30" s="15">
         <f t="shared" si="5"/>
-        <v>8.1112684775005981</v>
+        <v>8.0130482372500254</v>
       </c>
       <c r="H30" s="15">
         <f t="shared" si="5"/>
-        <v>7.7662449687511845</v>
+        <v>7.6209962709503252</v>
       </c>
       <c r="I30" s="15">
         <f t="shared" si="5"/>
-        <v>7.7917650587014835</v>
+        <v>7.6517678934506232</v>
       </c>
       <c r="J30" s="15">
         <f t="shared" si="5"/>
-        <v>7.8167421486511826</v>
+        <v>7.6814070209012089</v>
       </c>
       <c r="K30" s="15">
         <f t="shared" si="5"/>
-        <v>7.8410907149008837</v>
+        <v>7.7104176246517939</v>
       </c>
       <c r="L30" s="15">
         <f t="shared" si="5"/>
-        <v>7.8642677861011689</v>
+        <v>7.7382927333514937</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.35">
@@ -43176,31 +43190,31 @@
       </c>
       <c r="F31" s="15">
         <f>IF(F$22&lt;&gt;"",VLOOKUP(F29*1000000,'Powell-Elevation-Area'!$B$5:$D$689,3)*$B$18/1000000 + VLOOKUP(F30*1000000,'Mead-Elevation-Area'!$B$5:$D$676,3)*$C$18/1000000,"")</f>
-        <v>0.89561168849942696</v>
+        <v>0.89205216900057305</v>
       </c>
       <c r="G31" s="15">
         <f>IF(G$22&lt;&gt;"",VLOOKUP(G29*1000000,'Powell-Elevation-Area'!$B$5:$D$689,3)*$B$18/1000000 + VLOOKUP(G30*1000000,'Mead-Elevation-Area'!$B$5:$D$676,3)*$C$18/1000000,"")</f>
-        <v>0.87304701749882696</v>
+        <v>0.8671039325994</v>
       </c>
       <c r="H31" s="15">
         <f>IF(H$22&lt;&gt;"",VLOOKUP(H29*1000000,'Powell-Elevation-Area'!$B$5:$D$689,3)*$B$18/1000000 + VLOOKUP(H30*1000000,'Mead-Elevation-Area'!$B$5:$D$676,3)*$C$18/1000000,"")</f>
-        <v>0.85195982009939997</v>
+        <v>0.84145675499939998</v>
       </c>
       <c r="I31" s="15">
         <f>IF(I$22&lt;&gt;"",VLOOKUP(I29*1000000,'Powell-Elevation-Area'!$B$5:$D$689,3)*$B$18/1000000 + VLOOKUP(I30*1000000,'Mead-Elevation-Area'!$B$5:$D$676,3)*$C$18/1000000,"")</f>
-        <v>0.85304582010059993</v>
+        <v>0.84372174509882703</v>
       </c>
       <c r="J31" s="15">
         <f>IF(J$22&lt;&gt;"",VLOOKUP(J29*1000000,'Powell-Elevation-Area'!$B$5:$D$689,3)*$B$18/1000000 + VLOOKUP(J30*1000000,'Mead-Elevation-Area'!$B$5:$D$676,3)*$C$18/1000000,"")</f>
-        <v>0.85430286750060003</v>
+        <v>0.84497879249882701</v>
       </c>
       <c r="K31" s="15">
         <f>IF(K$22&lt;&gt;"",VLOOKUP(K29*1000000,'Powell-Elevation-Area'!$B$5:$D$689,3)*$B$18/1000000 + VLOOKUP(K30*1000000,'Mead-Elevation-Area'!$B$5:$D$676,3)*$C$18/1000000,"")</f>
-        <v>0.85664585759942702</v>
+        <v>0.84724978260060002</v>
       </c>
       <c r="L31" s="15">
         <f>IF(L$22&lt;&gt;"",VLOOKUP(L29*1000000,'Powell-Elevation-Area'!$B$5:$D$689,3)*$B$18/1000000 + VLOOKUP(L30*1000000,'Mead-Elevation-Area'!$B$5:$D$676,3)*$C$18/1000000,"")</f>
-        <v>0.85664585759942702</v>
+        <v>0.84961683000057309</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.35">
@@ -43222,31 +43236,31 @@
       </c>
       <c r="F32" s="15">
         <f t="shared" si="6"/>
-        <v>0.35653916962197557</v>
+        <v>0.35193280078489469</v>
       </c>
       <c r="G32" s="15">
         <f t="shared" si="6"/>
-        <v>0.34767189580454005</v>
+        <v>0.33896586499167913</v>
       </c>
       <c r="H32" s="15">
         <f t="shared" si="6"/>
-        <v>0.33939089570527925</v>
+        <v>0.3257685428262872</v>
       </c>
       <c r="I32" s="15">
         <f t="shared" si="6"/>
-        <v>0.36310324721401699</v>
+        <v>0.35065038871150594</v>
       </c>
       <c r="J32" s="15">
         <f t="shared" si="6"/>
-        <v>0.38553121854835831</v>
+        <v>0.37370770535527542</v>
       </c>
       <c r="K32" s="15">
         <f t="shared" si="6"/>
-        <v>0.40720926469428737</v>
+        <v>0.3958994060225336</v>
       </c>
       <c r="L32" s="15">
         <f t="shared" si="6"/>
-        <v>0.42658532362854812</v>
+        <v>0.41693578836138268</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.35">
@@ -43268,31 +43282,31 @@
       </c>
       <c r="F33" s="15">
         <f t="shared" si="6"/>
-        <v>0.53907251887745133</v>
+        <v>0.5401193682156783</v>
       </c>
       <c r="G33" s="15">
         <f t="shared" si="6"/>
-        <v>0.52537512169428702</v>
+        <v>0.52813806760772097</v>
       </c>
       <c r="H33" s="15">
         <f t="shared" si="6"/>
-        <v>0.51256892439412072</v>
+        <v>0.51568821217311267</v>
       </c>
       <c r="I33" s="15">
         <f t="shared" si="6"/>
-        <v>0.48994257288658294</v>
+        <v>0.49307135638732108</v>
       </c>
       <c r="J33" s="15">
         <f t="shared" si="6"/>
-        <v>0.46877164895224177</v>
+        <v>0.47127108714355159</v>
       </c>
       <c r="K33" s="15">
         <f t="shared" si="6"/>
-        <v>0.44943659290513965</v>
+        <v>0.45135037657806643</v>
       </c>
       <c r="L33" s="15">
         <f t="shared" si="6"/>
-        <v>0.4300605339708789</v>
+        <v>0.43268104163919041</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.35">
@@ -43652,31 +43666,31 @@
       </c>
       <c r="F45" s="15">
         <f>IF(F$22&lt;&gt;"",F25+F37-F32-F40,"")</f>
-        <v>9.1602708271803408</v>
+        <v>9.0648771960174219</v>
       </c>
       <c r="G45" s="15">
         <f t="shared" si="12"/>
-        <v>8.8875989313758001</v>
+        <v>8.7009113310257433</v>
       </c>
       <c r="H45" s="15">
         <f t="shared" si="12"/>
-        <v>8.6332080356705205</v>
+        <v>8.3601427881994557</v>
       </c>
       <c r="I45" s="15">
         <f t="shared" si="12"/>
-        <v>9.0551047884565037</v>
+        <v>8.7944923994879503</v>
       </c>
       <c r="J45" s="15">
         <f t="shared" si="12"/>
-        <v>9.4545735699081455</v>
+        <v>9.2057846941326744</v>
       </c>
       <c r="K45" s="15">
         <f t="shared" si="12"/>
-        <v>9.8323643052138578</v>
+        <v>9.5948852881101416</v>
       </c>
       <c r="L45" s="15">
         <f t="shared" si="12"/>
-        <v>10.190778981585311</v>
+        <v>9.9629494997487598</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.35">
@@ -43697,31 +43711,31 @@
       </c>
       <c r="F46" s="15">
         <f t="shared" si="13"/>
-        <v>17.229266127820857</v>
+        <v>17.22821927848263</v>
       </c>
       <c r="G46" s="15">
         <f t="shared" si="13"/>
-        <v>16.811891006126569</v>
+        <v>16.808081210874906</v>
       </c>
       <c r="H46" s="15">
         <f t="shared" si="13"/>
-        <v>16.417322081732447</v>
+        <v>16.410392998701791</v>
       </c>
       <c r="I46" s="15">
         <f t="shared" si="13"/>
-        <v>16.045379508845862</v>
+        <v>16.035321642314468</v>
       </c>
       <c r="J46" s="15">
         <f t="shared" si="13"/>
-        <v>15.694607859893623</v>
+        <v>15.682050555170914</v>
       </c>
       <c r="K46" s="15">
         <f t="shared" si="13"/>
-        <v>15.363171266988481</v>
+        <v>15.348700178592846</v>
       </c>
       <c r="L46" s="15">
         <f t="shared" si="13"/>
-        <v>15.051110733017602</v>
+        <v>15.034019136953656</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.35">
@@ -43796,13 +43810,13 @@
         <v>3.3</v>
       </c>
       <c r="E49" s="45">
-        <v>2.9</v>
+        <v>3</v>
       </c>
       <c r="F49" s="45">
-        <v>2.7</v>
+        <v>2.8</v>
       </c>
       <c r="G49" s="45">
-        <v>2.7</v>
+        <v>2.8</v>
       </c>
       <c r="H49" s="26">
         <v>2</v>
@@ -44050,35 +44064,35 @@
       </c>
       <c r="E54" s="15">
         <f t="shared" si="19"/>
-        <v>6.7418099968023153</v>
+        <v>6.6418099968023157</v>
       </c>
       <c r="F54" s="15">
         <f t="shared" si="19"/>
-        <v>6.4602708271803406</v>
+        <v>6.2648771960174221</v>
       </c>
       <c r="G54" s="15">
         <f t="shared" si="19"/>
-        <v>6.1875989313758</v>
+        <v>5.9009113310257435</v>
       </c>
       <c r="H54" s="15">
         <f t="shared" si="19"/>
-        <v>6.6332080356705205</v>
+        <v>6.3601427881994557</v>
       </c>
       <c r="I54" s="15">
         <f t="shared" si="19"/>
-        <v>7.0551047884565037</v>
+        <v>6.7944923994879503</v>
       </c>
       <c r="J54" s="15">
         <f t="shared" si="19"/>
-        <v>7.4545735699081455</v>
+        <v>7.2057846941326744</v>
       </c>
       <c r="K54" s="15">
         <f t="shared" si="19"/>
-        <v>7.8323643052138578</v>
+        <v>7.5948852881101416</v>
       </c>
       <c r="L54" s="15">
         <f t="shared" si="19"/>
-        <v>8.1907789815853107</v>
+        <v>7.9629494997487598</v>
       </c>
       <c r="N54" s="41">
         <v>1040</v>
@@ -44115,31 +44129,31 @@
       </c>
       <c r="F55" s="15">
         <f t="shared" si="20"/>
-        <v>9.7622661278208565</v>
+        <v>9.7612192784826295</v>
       </c>
       <c r="G55" s="15">
         <f t="shared" si="20"/>
-        <v>9.3448910061265682</v>
+        <v>9.3410812108749059</v>
       </c>
       <c r="H55" s="15">
         <f t="shared" si="20"/>
-        <v>8.9503220817324465</v>
+        <v>8.9433929987017908</v>
       </c>
       <c r="I55" s="15">
         <f t="shared" si="20"/>
-        <v>8.5783795088458614</v>
+        <v>8.5683216423144675</v>
       </c>
       <c r="J55" s="15">
         <f t="shared" si="20"/>
-        <v>8.227607859893622</v>
+        <v>8.2150505551709134</v>
       </c>
       <c r="K55" s="15">
         <f t="shared" si="20"/>
-        <v>7.89617126698848</v>
+        <v>7.8817001785928458</v>
       </c>
       <c r="L55" s="15">
         <f t="shared" si="20"/>
-        <v>7.5841107330176012</v>
+        <v>7.5670191369536557</v>
       </c>
       <c r="N55" s="41">
         <v>1045</v>
@@ -44234,35 +44248,35 @@
       </c>
       <c r="E57" s="15">
         <f t="shared" si="22"/>
-        <v>16.935148643500622</v>
+        <v>16.835148643500624</v>
       </c>
       <c r="F57" s="15">
         <f t="shared" si="22"/>
-        <v>16.222536955001196</v>
+        <v>16.026096474500051</v>
       </c>
       <c r="G57" s="15">
         <f t="shared" si="22"/>
-        <v>15.532489937502369</v>
+        <v>15.24199254190065</v>
       </c>
       <c r="H57" s="15">
         <f t="shared" si="22"/>
-        <v>15.583530117402967</v>
+        <v>15.303535786901246</v>
       </c>
       <c r="I57" s="15">
         <f t="shared" si="22"/>
-        <v>15.633484297302365</v>
+        <v>15.362814041802418</v>
       </c>
       <c r="J57" s="15">
         <f t="shared" si="22"/>
-        <v>15.682181429801767</v>
+        <v>15.420835249303588</v>
       </c>
       <c r="K57" s="15">
         <f t="shared" si="22"/>
-        <v>15.728535572202338</v>
+        <v>15.476585466702987</v>
       </c>
       <c r="L57" s="15">
         <f t="shared" si="22"/>
-        <v>15.774889714602912</v>
+        <v>15.529968636702415</v>
       </c>
       <c r="N57" s="41">
         <v>1075</v>
@@ -44283,7 +44297,7 @@
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B58" s="1"/>
       <c r="C58" s="15">
@@ -44296,35 +44310,35 @@
       </c>
       <c r="E58" s="15">
         <f t="shared" si="23"/>
-        <v>8.174504903219125</v>
+        <v>8.1245049032191226</v>
       </c>
       <c r="F58" s="15">
         <f t="shared" si="23"/>
-        <v>8.2997666746277403</v>
+        <v>8.2525932837153917</v>
       </c>
       <c r="G58" s="15">
         <f t="shared" si="23"/>
-        <v>8.2973516129448726</v>
+        <v>8.2530861013080212</v>
       </c>
       <c r="H58" s="15">
         <f t="shared" si="23"/>
-        <v>8.6350890143444232</v>
+        <v>8.6434598346734131</v>
       </c>
       <c r="I58" s="15">
         <f t="shared" si="23"/>
-        <v>8.6119196628362822</v>
+        <v>8.6197104838379097</v>
       </c>
       <c r="J58" s="15">
         <f t="shared" si="23"/>
-        <v>8.5901202152019422</v>
+        <v>8.597281690894139</v>
       </c>
       <c r="K58" s="15">
         <f t="shared" si="23"/>
-        <v>8.5696136641054252</v>
+        <v>8.5762254852777673</v>
       </c>
       <c r="L58" s="15">
         <f t="shared" si="23"/>
-        <v>8.5502376051711657</v>
+        <v>8.556372626638904</v>
       </c>
       <c r="N58" s="41">
         <v>1090</v>
@@ -44398,43 +44412,43 @@
         <v>132</v>
       </c>
       <c r="C61" s="15">
-        <f>IF(C$22&lt;&gt;"",C50+C60,"")</f>
+        <f t="shared" ref="C61:L61" si="25">IF(C$22&lt;&gt;"",C50+C60,"")</f>
         <v>7.0670000000000002</v>
       </c>
       <c r="D61" s="15">
-        <f>IF(D$22&lt;&gt;"",D50+D60,"")</f>
+        <f t="shared" si="25"/>
         <v>7.0670000000000002</v>
       </c>
       <c r="E61" s="15">
-        <f>IF(E$22&lt;&gt;"",E50+E60,"")</f>
+        <f t="shared" si="25"/>
         <v>7.0670000000000002</v>
       </c>
       <c r="F61" s="15">
-        <f>IF(F$22&lt;&gt;"",F50+F60,"")</f>
+        <f t="shared" si="25"/>
         <v>7.0670000000000002</v>
       </c>
       <c r="G61" s="15">
-        <f>IF(G$22&lt;&gt;"",G50+G60,"")</f>
+        <f t="shared" si="25"/>
         <v>7.0670000000000002</v>
       </c>
       <c r="H61" s="15">
-        <f>IF(H$22&lt;&gt;"",H50+H60,"")</f>
+        <f t="shared" si="25"/>
         <v>7.0670000000000002</v>
       </c>
       <c r="I61" s="15">
-        <f>IF(I$22&lt;&gt;"",I50+I60,"")</f>
+        <f t="shared" si="25"/>
         <v>7.0670000000000002</v>
       </c>
       <c r="J61" s="15">
-        <f>IF(J$22&lt;&gt;"",J50+J60,"")</f>
+        <f t="shared" si="25"/>
         <v>7.0670000000000002</v>
       </c>
       <c r="K61" s="15">
-        <f>IF(K$22&lt;&gt;"",K50+K60,"")</f>
+        <f t="shared" si="25"/>
         <v>7.0670000000000002</v>
       </c>
       <c r="L61" s="15">
-        <f>IF(L$22&lt;&gt;"",L50+L60,"")</f>
+        <f t="shared" si="25"/>
         <v>7.0670000000000002</v>
       </c>
     </row>
@@ -44569,8 +44583,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6E878AF-96FE-424D-B802-94EDCA32030C}">
   <dimension ref="A1:R63"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C59" sqref="C59:G59"/>
+    <sheetView topLeftCell="A37" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -44633,48 +44647,48 @@
         <v>53</v>
       </c>
       <c r="B5" s="50"/>
-      <c r="C5" s="64"/>
-      <c r="D5" s="64"/>
-      <c r="E5" s="64"/>
-      <c r="F5" s="64"/>
-      <c r="G5" s="64"/>
-      <c r="H5" s="64"/>
+      <c r="C5" s="66"/>
+      <c r="D5" s="66"/>
+      <c r="E5" s="66"/>
+      <c r="F5" s="66"/>
+      <c r="G5" s="66"/>
+      <c r="H5" s="66"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="17" t="s">
         <v>41</v>
       </c>
       <c r="B6" s="50"/>
-      <c r="C6" s="64"/>
-      <c r="D6" s="64"/>
-      <c r="E6" s="64"/>
-      <c r="F6" s="64"/>
-      <c r="G6" s="64"/>
-      <c r="H6" s="64"/>
+      <c r="C6" s="66"/>
+      <c r="D6" s="66"/>
+      <c r="E6" s="66"/>
+      <c r="F6" s="66"/>
+      <c r="G6" s="66"/>
+      <c r="H6" s="66"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="17" t="s">
         <v>42</v>
       </c>
       <c r="B7" s="50"/>
-      <c r="C7" s="64"/>
-      <c r="D7" s="64"/>
-      <c r="E7" s="64"/>
-      <c r="F7" s="64"/>
-      <c r="G7" s="64"/>
-      <c r="H7" s="64"/>
+      <c r="C7" s="66"/>
+      <c r="D7" s="66"/>
+      <c r="E7" s="66"/>
+      <c r="F7" s="66"/>
+      <c r="G7" s="66"/>
+      <c r="H7" s="66"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="17" t="s">
         <v>43</v>
       </c>
       <c r="B8" s="50"/>
-      <c r="C8" s="64"/>
-      <c r="D8" s="64"/>
-      <c r="E8" s="64"/>
-      <c r="F8" s="64"/>
-      <c r="G8" s="64"/>
-      <c r="H8" s="64"/>
+      <c r="C8" s="66"/>
+      <c r="D8" s="66"/>
+      <c r="E8" s="66"/>
+      <c r="F8" s="66"/>
+      <c r="G8" s="66"/>
+      <c r="H8" s="66"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="17"/>
@@ -44737,7 +44751,7 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B19" s="12">
         <v>11</v>
@@ -46276,7 +46290,7 @@
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B58" s="1"/>
       <c r="C58" s="15">
@@ -46391,43 +46405,43 @@
         <v>132</v>
       </c>
       <c r="C61" s="15">
-        <f>IF(C$22&lt;&gt;"",C50+C60,"")</f>
+        <f t="shared" ref="C61:L61" si="26">IF(C$22&lt;&gt;"",C50+C60,"")</f>
         <v>7.0670000000000002</v>
       </c>
       <c r="D61" s="15">
-        <f>IF(D$22&lt;&gt;"",D50+D60,"")</f>
+        <f t="shared" si="26"/>
         <v>7.0670000000000002</v>
       </c>
       <c r="E61" s="15">
-        <f>IF(E$22&lt;&gt;"",E50+E60,"")</f>
+        <f t="shared" si="26"/>
         <v>6.9829999999999997</v>
       </c>
       <c r="F61" s="15">
-        <f>IF(F$22&lt;&gt;"",F50+F60,"")</f>
+        <f t="shared" si="26"/>
         <v>6.9829999999999997</v>
       </c>
       <c r="G61" s="15">
-        <f>IF(G$22&lt;&gt;"",G50+G60,"")</f>
+        <f t="shared" si="26"/>
         <v>6.9829999999999997</v>
       </c>
       <c r="H61" s="15">
-        <f>IF(H$22&lt;&gt;"",H50+H60,"")</f>
+        <f t="shared" si="26"/>
         <v>6.9829999999999997</v>
       </c>
       <c r="I61" s="15">
-        <f>IF(I$22&lt;&gt;"",I50+I60,"")</f>
+        <f t="shared" si="26"/>
         <v>6.9829999999999997</v>
       </c>
       <c r="J61" s="15">
-        <f>IF(J$22&lt;&gt;"",J50+J60,"")</f>
+        <f t="shared" si="26"/>
         <v>6.9829999999999997</v>
       </c>
       <c r="K61" s="15">
-        <f>IF(K$22&lt;&gt;"",K50+K60,"")</f>
+        <f t="shared" si="26"/>
         <v>6.9829999999999997</v>
       </c>
       <c r="L61" s="15">
-        <f>IF(L$22&lt;&gt;"",L50+L60,"")</f>
+        <f t="shared" si="26"/>
         <v>6.9829999999999997</v>
       </c>
     </row>
@@ -46526,10 +46540,10 @@
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="7:16" ht="36" x14ac:dyDescent="0.8">
-      <c r="G1" s="65" t="s">
+      <c r="G1" s="53" t="s">
         <v>41</v>
       </c>
-      <c r="P1" s="65" t="s">
+      <c r="P1" s="53" t="s">
         <v>42</v>
       </c>
     </row>
@@ -46607,58 +46621,58 @@
         <v>53</v>
       </c>
       <c r="B5" s="36" t="s">
-        <v>157</v>
-      </c>
-      <c r="C5" s="64" t="s">
-        <v>158</v>
-      </c>
-      <c r="D5" s="64"/>
-      <c r="E5" s="64"/>
-      <c r="F5" s="64"/>
-      <c r="G5" s="64"/>
-      <c r="H5" s="64"/>
+        <v>153</v>
+      </c>
+      <c r="C5" s="66" t="s">
+        <v>154</v>
+      </c>
+      <c r="D5" s="66"/>
+      <c r="E5" s="66"/>
+      <c r="F5" s="66"/>
+      <c r="G5" s="66"/>
+      <c r="H5" s="66"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="17" t="s">
         <v>41</v>
       </c>
       <c r="B6" s="36" t="s">
-        <v>157</v>
-      </c>
-      <c r="C6" s="64"/>
-      <c r="D6" s="64"/>
-      <c r="E6" s="64"/>
-      <c r="F6" s="64"/>
-      <c r="G6" s="64"/>
-      <c r="H6" s="64"/>
+        <v>153</v>
+      </c>
+      <c r="C6" s="66"/>
+      <c r="D6" s="66"/>
+      <c r="E6" s="66"/>
+      <c r="F6" s="66"/>
+      <c r="G6" s="66"/>
+      <c r="H6" s="66"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="17" t="s">
         <v>42</v>
       </c>
       <c r="B7" s="36" t="s">
-        <v>157</v>
-      </c>
-      <c r="C7" s="64"/>
-      <c r="D7" s="64"/>
-      <c r="E7" s="64"/>
-      <c r="F7" s="64"/>
-      <c r="G7" s="64"/>
-      <c r="H7" s="64"/>
+        <v>153</v>
+      </c>
+      <c r="C7" s="66"/>
+      <c r="D7" s="66"/>
+      <c r="E7" s="66"/>
+      <c r="F7" s="66"/>
+      <c r="G7" s="66"/>
+      <c r="H7" s="66"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="17" t="s">
         <v>43</v>
       </c>
       <c r="B8" s="36" t="s">
-        <v>157</v>
-      </c>
-      <c r="C8" s="64"/>
-      <c r="D8" s="64"/>
-      <c r="E8" s="64"/>
-      <c r="F8" s="64"/>
-      <c r="G8" s="64"/>
-      <c r="H8" s="64"/>
+        <v>153</v>
+      </c>
+      <c r="C8" s="66"/>
+      <c r="D8" s="66"/>
+      <c r="E8" s="66"/>
+      <c r="F8" s="66"/>
+      <c r="G8" s="66"/>
+      <c r="H8" s="66"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="17"/>
@@ -46693,7 +46707,7 @@
         <v>55</v>
       </c>
       <c r="D15" s="67" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="E15" s="68"/>
       <c r="F15" s="68"/>
@@ -46728,7 +46742,7 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B19" s="12">
         <v>11</v>
@@ -47206,7 +47220,7 @@
       <c r="A32" t="s">
         <v>104</v>
       </c>
-      <c r="B32" s="66">
+      <c r="B32" s="54">
         <f>+D30-C30-C23+SUM(C50:C52)+C33+C34</f>
         <v>8.5867059736492894</v>
       </c>
@@ -48274,7 +48288,7 @@
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B58" s="1"/>
       <c r="C58" s="15">
@@ -48382,43 +48396,43 @@
         <v>132</v>
       </c>
       <c r="C61" s="15">
-        <f>IF(C$22&lt;&gt;"",C50+C60,"")</f>
+        <f t="shared" ref="C61:L61" si="26">IF(C$22&lt;&gt;"",C50+C60,"")</f>
         <v>7.0670000000000002</v>
       </c>
       <c r="D61" s="15">
-        <f>IF(D$22&lt;&gt;"",D50+D60,"")</f>
+        <f t="shared" si="26"/>
         <v>7.0670000000000002</v>
       </c>
       <c r="E61" s="15">
-        <f>IF(E$22&lt;&gt;"",E50+E60,"")</f>
+        <f t="shared" si="26"/>
         <v>6.9829999999999997</v>
       </c>
       <c r="F61" s="15">
-        <f>IF(F$22&lt;&gt;"",F50+F60,"")</f>
+        <f t="shared" si="26"/>
         <v>6.9829999999999997</v>
       </c>
       <c r="G61" s="15">
-        <f>IF(G$22&lt;&gt;"",G50+G60,"")</f>
+        <f t="shared" si="26"/>
         <v>6.9829999999999997</v>
       </c>
       <c r="H61" s="15">
-        <f>IF(H$22&lt;&gt;"",H50+H60,"")</f>
+        <f t="shared" si="26"/>
         <v>6.9829999999999997</v>
       </c>
       <c r="I61" s="15">
-        <f>IF(I$22&lt;&gt;"",I50+I60,"")</f>
+        <f t="shared" si="26"/>
         <v>6.9829999999999997</v>
       </c>
       <c r="J61" s="15">
-        <f>IF(J$22&lt;&gt;"",J50+J60,"")</f>
+        <f t="shared" si="26"/>
         <v>6.9829999999999997</v>
       </c>
       <c r="K61" s="15">
-        <f>IF(K$22&lt;&gt;"",K50+K60,"")</f>
+        <f t="shared" si="26"/>
         <v>6.9829999999999997</v>
       </c>
       <c r="L61" s="15">
-        <f>IF(L$22&lt;&gt;"",L50+L60,"")</f>
+        <f t="shared" si="26"/>
         <v>6.7330000000000005</v>
       </c>
     </row>
@@ -48453,8 +48467,8 @@
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="7:16" ht="36" x14ac:dyDescent="0.8">
-      <c r="G1" s="65"/>
-      <c r="P1" s="65"/>
+      <c r="G1" s="53"/>
+      <c r="P1" s="53"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>